<commit_message>
[ADD] add satellogic data processing to data_loading.py
</commit_message>
<xml_diff>
--- a/financial_data/satellogic.xlsx
+++ b/financial_data/satellogic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\OneDrive\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F08FBDF-5F6A-4118-9BDB-EB3A9C056E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E0C7EE-E514-42E1-A11E-A287F05FF94C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{84ACD714-4695-47C3-B1A3-494310BA187C}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{84ACD714-4695-47C3-B1A3-494310BA187C}"/>
   </bookViews>
   <sheets>
     <sheet name="consolidated" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>Revenue</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Contract liabilities, non-current</t>
+  </si>
+  <si>
+    <t>Quarter</t>
   </si>
 </sst>
 </file>
@@ -584,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28921E86-815C-4D28-B61B-DA9A063C903A}">
   <dimension ref="A1:AB3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,6 +613,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>46</v>
+      </c>
       <c r="B1" s="3" t="s">
         <v>19</v>
       </c>
@@ -873,7 +879,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC2D95B-D178-464E-A9C5-854655F43FD1}">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -898,8 +906,10 @@
     <col min="20" max="20" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="8" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
+    <row r="1" spans="1:20" s="8" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>46</v>
+      </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
[FIX] update satellogic consolidated data with interpolation
</commit_message>
<xml_diff>
--- a/financial_data/satellogic.xlsx
+++ b/financial_data/satellogic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF27C5B4-2E60-4F78-8F2C-37D565E28D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C1E61B-22CF-4AFD-A4A9-914BE524A99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{84ACD714-4695-47C3-B1A3-494310BA187C}"/>
   </bookViews>
@@ -224,12 +224,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -244,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -265,6 +271,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -600,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28921E86-815C-4D28-B61B-DA9A063C903A}">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -800,88 +809,427 @@
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="9">
+        <v>44681</v>
+      </c>
+      <c r="B3" s="4">
+        <f>(0.25*(B$6-B$2))+B$2</f>
+        <v>25531750</v>
+      </c>
+      <c r="C3" s="4">
+        <f t="shared" ref="C3:AB3" si="0">(0.25*(C6-C2))+C2</f>
+        <v>31500</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" si="0"/>
+        <v>1244000</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" si="0"/>
+        <v>2820750</v>
+      </c>
+      <c r="F3" s="4">
+        <f t="shared" si="0"/>
+        <v>29628000</v>
+      </c>
+      <c r="G3" s="4">
+        <f t="shared" si="0"/>
+        <v>36392750</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" si="0"/>
+        <v>1230000</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="shared" si="0"/>
+        <v>4259000</v>
+      </c>
+      <c r="J3" s="4">
+        <f t="shared" si="0"/>
+        <v>1892500</v>
+      </c>
+      <c r="K3" s="4">
+        <f t="shared" si="0"/>
+        <v>73402250</v>
+      </c>
+      <c r="L3" s="4">
+        <f t="shared" si="0"/>
+        <v>7450000</v>
+      </c>
+      <c r="M3" s="4">
+        <f t="shared" si="0"/>
+        <v>19180500</v>
+      </c>
+      <c r="N3" s="4">
+        <f t="shared" si="0"/>
+        <v>81354750</v>
+      </c>
+      <c r="O3" s="4">
+        <f t="shared" si="0"/>
+        <v>109511500</v>
+      </c>
+      <c r="P3" s="4">
+        <f t="shared" si="0"/>
+        <v>338250</v>
+      </c>
+      <c r="Q3" s="4">
+        <f t="shared" si="0"/>
+        <v>1186500</v>
+      </c>
+      <c r="R3" s="4">
+        <f t="shared" si="0"/>
+        <v>1282750</v>
+      </c>
+      <c r="S3" s="4">
+        <f t="shared" si="0"/>
+        <v>220304250</v>
+      </c>
+      <c r="T3" s="4">
+        <f>(0.25*(T6-T2))+T2</f>
+        <v>1000000</v>
+      </c>
+      <c r="U3" s="4">
+        <f t="shared" si="0"/>
+        <v>3078000</v>
+      </c>
+      <c r="V3" s="4">
+        <f t="shared" si="0"/>
+        <v>2044500</v>
+      </c>
+      <c r="W3" s="4">
+        <f t="shared" si="0"/>
+        <v>226426750</v>
+      </c>
+      <c r="X3" s="4">
+        <f t="shared" si="0"/>
+        <v>156835250</v>
+      </c>
+      <c r="Y3" s="4">
+        <f t="shared" si="0"/>
+        <v>-142500</v>
+      </c>
+      <c r="Z3" s="4">
+        <f t="shared" si="0"/>
+        <v>-195334250</v>
+      </c>
+      <c r="AA3" s="4">
+        <f t="shared" si="0"/>
+        <v>-169004000</v>
+      </c>
+      <c r="AB3" s="4">
+        <f t="shared" si="0"/>
+        <v>73402250</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>44742</v>
+      </c>
+      <c r="B4" s="4">
+        <f>(0.5*(B$6-B$2))+B$2</f>
+        <v>42530500</v>
+      </c>
+      <c r="C4" s="4">
+        <f t="shared" ref="C4:AB4" si="1">(0.5*(C$6-C$2))+C$2</f>
+        <v>63000</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="1"/>
+        <v>1292000</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="1"/>
+        <v>2946500</v>
+      </c>
+      <c r="F4" s="4">
+        <f t="shared" si="1"/>
+        <v>46832000</v>
+      </c>
+      <c r="G4" s="4">
+        <f t="shared" si="1"/>
+        <v>40255500</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="1"/>
+        <v>820000</v>
+      </c>
+      <c r="I4" s="4">
+        <f t="shared" si="1"/>
+        <v>5563000</v>
+      </c>
+      <c r="J4" s="4">
+        <f t="shared" si="1"/>
+        <v>3416000</v>
+      </c>
+      <c r="K4" s="4">
+        <f t="shared" si="1"/>
+        <v>96886500</v>
+      </c>
+      <c r="L4" s="4">
+        <f t="shared" si="1"/>
+        <v>8250000</v>
+      </c>
+      <c r="M4" s="4">
+        <f t="shared" si="1"/>
+        <v>14926000</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" si="1"/>
+        <v>54236500</v>
+      </c>
+      <c r="O4" s="4">
+        <f t="shared" si="1"/>
+        <v>75786000</v>
+      </c>
+      <c r="P4" s="4">
+        <f t="shared" si="1"/>
+        <v>676500</v>
+      </c>
+      <c r="Q4" s="4">
+        <f t="shared" si="1"/>
+        <v>1438000</v>
+      </c>
+      <c r="R4" s="4">
+        <f t="shared" si="1"/>
+        <v>1580500</v>
+      </c>
+      <c r="S4" s="4">
+        <f t="shared" si="1"/>
+        <v>156893500</v>
+      </c>
+      <c r="T4" s="4">
+        <f t="shared" si="1"/>
+        <v>1000000</v>
+      </c>
+      <c r="U4" s="4">
+        <f t="shared" si="1"/>
+        <v>4073000</v>
+      </c>
+      <c r="V4" s="4">
+        <f t="shared" si="1"/>
+        <v>1537000</v>
+      </c>
+      <c r="W4" s="4">
+        <f t="shared" si="1"/>
+        <v>163503500</v>
+      </c>
+      <c r="X4" s="4">
+        <f t="shared" si="1"/>
+        <v>217199500</v>
+      </c>
+      <c r="Y4" s="4">
+        <f t="shared" si="1"/>
+        <v>-199000</v>
+      </c>
+      <c r="Z4" s="4">
+        <f t="shared" si="1"/>
+        <v>-204494500</v>
+      </c>
+      <c r="AA4" s="4">
+        <f t="shared" si="1"/>
+        <v>-77270000</v>
+      </c>
+      <c r="AB4" s="4">
+        <f t="shared" si="1"/>
+        <v>96886500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>44834</v>
+      </c>
+      <c r="B5" s="4">
+        <f>(0.75*(B$6-B$2))+B$2</f>
+        <v>59529250</v>
+      </c>
+      <c r="C5" s="4">
+        <f t="shared" ref="C5:AB5" si="2">(0.75*(C$6-C$2))+C$2</f>
+        <v>94500</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="2"/>
+        <v>1340000</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="2"/>
+        <v>3072250</v>
+      </c>
+      <c r="F5" s="4">
+        <f t="shared" si="2"/>
+        <v>64036000</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" si="2"/>
+        <v>44118250</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="2"/>
+        <v>410000</v>
+      </c>
+      <c r="I5" s="4">
+        <f t="shared" si="2"/>
+        <v>6867000</v>
+      </c>
+      <c r="J5" s="4">
+        <f t="shared" si="2"/>
+        <v>4939500</v>
+      </c>
+      <c r="K5" s="4">
+        <f t="shared" si="2"/>
+        <v>120370750</v>
+      </c>
+      <c r="L5" s="4">
+        <f t="shared" si="2"/>
+        <v>9050000</v>
+      </c>
+      <c r="M5" s="4">
+        <f t="shared" si="2"/>
+        <v>10671500</v>
+      </c>
+      <c r="N5" s="4">
+        <f t="shared" si="2"/>
+        <v>27118250</v>
+      </c>
+      <c r="O5" s="4">
+        <f t="shared" si="2"/>
+        <v>42060500</v>
+      </c>
+      <c r="P5" s="4">
+        <f t="shared" si="2"/>
+        <v>1014750</v>
+      </c>
+      <c r="Q5" s="4">
+        <f t="shared" si="2"/>
+        <v>1689500</v>
+      </c>
+      <c r="R5" s="4">
+        <f t="shared" si="2"/>
+        <v>1878250</v>
+      </c>
+      <c r="S5" s="4">
+        <f t="shared" si="2"/>
+        <v>93482750</v>
+      </c>
+      <c r="T5" s="4">
+        <f t="shared" si="2"/>
+        <v>1000000</v>
+      </c>
+      <c r="U5" s="4">
+        <f t="shared" si="2"/>
+        <v>5068000</v>
+      </c>
+      <c r="V5" s="4">
+        <f t="shared" si="2"/>
+        <v>1029500</v>
+      </c>
+      <c r="W5" s="4">
+        <f t="shared" si="2"/>
+        <v>100580250</v>
+      </c>
+      <c r="X5" s="4">
+        <f t="shared" si="2"/>
+        <v>277563750</v>
+      </c>
+      <c r="Y5" s="4">
+        <f t="shared" si="2"/>
+        <v>-255500</v>
+      </c>
+      <c r="Z5" s="4">
+        <f t="shared" si="2"/>
+        <v>-213654750</v>
+      </c>
+      <c r="AA5" s="4">
+        <f t="shared" si="2"/>
+        <v>14464000</v>
+      </c>
+      <c r="AB5" s="4">
+        <f t="shared" si="2"/>
+        <v>120370750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>44926</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B6" s="4">
         <v>76528000</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C6" s="4">
         <v>126000</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D6" s="4">
         <v>1388000</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E6" s="4">
         <v>3198000</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F6" s="4">
         <v>81240000</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G6" s="4">
         <v>47981000</v>
       </c>
-      <c r="H3" s="4">
-        <v>0</v>
-      </c>
-      <c r="I3" s="4">
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4">
         <v>8171000</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J6" s="4">
         <v>6463000</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K6" s="4">
         <v>143855000</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L6" s="4">
         <v>9850000</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M6" s="4">
         <v>6417000</v>
       </c>
-      <c r="N3" s="4">
-        <v>0</v>
-      </c>
-      <c r="O3" s="4">
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
         <v>8335000</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P6" s="4">
         <v>1353000</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="Q6" s="4">
         <v>1941000</v>
       </c>
-      <c r="R3" s="4">
+      <c r="R6" s="4">
         <v>2176000</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S6" s="4">
         <v>30072000</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T6" s="4">
         <v>1000000</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U6" s="4">
         <v>6063000</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V6" s="4">
         <v>522000</v>
       </c>
-      <c r="W3" s="4">
+      <c r="W6" s="4">
         <v>37657000</v>
       </c>
-      <c r="X3" s="4">
+      <c r="X6" s="4">
         <v>337928000</v>
       </c>
-      <c r="Y3" s="4">
+      <c r="Y6" s="4">
         <v>-312000</v>
       </c>
-      <c r="Z3" s="4">
+      <c r="Z6" s="4">
         <v>-222815000</v>
       </c>
-      <c r="AA3" s="4">
+      <c r="AA6" s="4">
         <v>106198000</v>
       </c>
-      <c r="AB3" s="4">
+      <c r="AB6" s="4">
         <v>143855000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new satellogic data 20240713
</commit_message>
<xml_diff>
--- a/financial_data/satellogic.xlsx
+++ b/financial_data/satellogic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shinten/Desktop/untitled folder/space_econometrics/financial_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28E2C35-5D4E-3A4F-BE6D-BE97702C8F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC41777A-F87D-6B4F-B2B9-D1A83F071918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="500" windowWidth="28800" windowHeight="15720" xr2:uid="{84ACD714-4695-47C3-B1A3-494310BA187C}"/>
+    <workbookView xWindow="1040" yWindow="640" windowWidth="28800" windowHeight="15720" xr2:uid="{84ACD714-4695-47C3-B1A3-494310BA187C}"/>
   </bookViews>
   <sheets>
     <sheet name="consolidated" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="46">
   <si>
     <t>Revenue</t>
   </si>
@@ -62,260 +62,118 @@
     <t>Debt</t>
   </si>
   <si>
-    <t>ResfI·icted cash</t>
-    <phoneticPr fontId="1"/>
+    <t>Prepaid expenses and other currentassets</t>
+  </si>
+  <si>
+    <t>Operating lease liabilities</t>
+  </si>
+  <si>
+    <t>Accumulated other comprehensive loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total costs and expenses </t>
+  </si>
+  <si>
+    <t>Finance income (expense), net</t>
+  </si>
+  <si>
+    <t>Total other income (expense), net</t>
+  </si>
+  <si>
+    <t>Foreign currency translation gain (loss), netoftax</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Restricted cash</t>
   </si>
   <si>
     <t>Accounts receivable</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Prepaid expenses and other currentassets</t>
-  </si>
-  <si>
-    <t>Total current assets</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Propertyand equipment,net</t>
-  </si>
-  <si>
-    <t>Other non-currentassets</t>
-  </si>
-  <si>
-    <t>Total assets</t>
+  </si>
+  <si>
+    <t>Total Current Assets</t>
+  </si>
+  <si>
+    <t>Property and equipment,net</t>
+  </si>
+  <si>
+    <t>Other non-current assets</t>
+  </si>
+  <si>
+    <t>Total Assets</t>
   </si>
   <si>
     <t>Accounts payable</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Warrant liabilities</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Earnout liabilities</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Operating lease liabilities</t>
-  </si>
-  <si>
-    <t>Contractliabilities</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Total current liabilities</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Conu·actliabilities</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Operating lease liabilities (current liabilities)</t>
+  </si>
+  <si>
+    <t>Contract liabilities (current liabilities)</t>
+  </si>
+  <si>
+    <t>Total Current Liabilities</t>
+  </si>
+  <si>
+    <t>Contract liabilities</t>
   </si>
   <si>
     <t>Other non-current liabilities</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Total liabilities</t>
+  </si>
+  <si>
+    <t>Total Liabilities</t>
   </si>
   <si>
     <t>Treasury stock, at cost</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Accumulated other comprehensive loss</t>
-  </si>
-  <si>
-    <t>Total stockholders' equity</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Total liabilities and stockholders'equity</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>Cost</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>of</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>sales</t>
-    </r>
+  </si>
+  <si>
+    <t>Total Equity</t>
+  </si>
+  <si>
+    <t>Liabilities and Equity</t>
+  </si>
+  <si>
+    <t>Cost of sales</t>
   </si>
   <si>
     <t>General and administrative expenses</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Research and development</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>Depreciation expense</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>Other</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>operating</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>expenses</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Total costs and expenses </t>
-  </si>
-  <si>
-    <t>Operating loss</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Finance income (expense), net</t>
+  </si>
+  <si>
+    <t>Other operating expenses</t>
+  </si>
+  <si>
+    <t>Total operating expenses</t>
   </si>
   <si>
     <t>Change in fair value offinancial instrnments</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> Loss on extinguishment</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>of</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color indexed="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>debt</t>
-    </r>
-  </si>
-  <si>
-    <t>Total other income (expense), net</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Loss on extinguishment of debt</t>
   </si>
   <si>
     <t>Loss before income tax</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>Income tax (expense)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  benefit </t>
-    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Income tax (expense)  benefit </t>
   </si>
   <si>
     <t>Net loss available to stockholders Other comprehensive loss</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Foreign currency translation gain (loss), netoftax</t>
-  </si>
-  <si>
-    <t>Comprehensive loss</t>
-  </si>
-  <si>
-    <t>-</t>
+  </si>
+  <si>
+    <t>Net loss</t>
   </si>
 </sst>
 </file>
@@ -323,10 +181,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="167" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,12 +214,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -385,7 +237,7 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -394,19 +246,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -745,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28921E86-815C-4D28-B61B-DA9A063C903A}">
   <dimension ref="A1:AT18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -796,136 +648,136 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="U1" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="V1" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="X1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="Y1" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="Z1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="AA1" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="AB1" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="AC1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="AD1" s="5" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="AG1" s="5" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="AH1" s="5" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="AI1" s="5" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="AJ1" s="4" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="AK1" s="5" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="AL1" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="AM1" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="AN1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="AO1" s="5" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="AP1" s="4" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="AQ1" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="AR1" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="AS1" s="4" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="AT1" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
@@ -933,91 +785,91 @@
         <v>43830</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Z2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AA2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AB2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AC2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AD2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AE2" s="7">
         <v>-4324000</v>
@@ -1032,7 +884,7 @@
         <v>-5763000</v>
       </c>
       <c r="AI2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AJ2" s="7">
         <v>-20697000</v>
@@ -1041,16 +893,16 @@
         <v>-4103000</v>
       </c>
       <c r="AL2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AM2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN2" s="7">
         <v>-112000</v>
       </c>
       <c r="AO2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AP2" s="7">
         <v>-20682000</v>
@@ -1062,7 +914,7 @@
         <v>-20765000</v>
       </c>
       <c r="AS2" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AT2" s="7">
         <v>-20765000</v>
@@ -1073,149 +925,138 @@
         <v>43920</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="N3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Q3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="R3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="S3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="T3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="V3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="X3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Y3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Z3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AA3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AB3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AC3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AD3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AE3" s="8">
-        <f t="shared" ref="AE3:AH3" si="0">(AE2-AE4)/($A4-$A2)*($A4-$A3)+AE4</f>
         <v>-5228672.1311475411</v>
       </c>
       <c r="AF3" s="8">
-        <f t="shared" si="0"/>
         <v>-6106918.0327868853</v>
       </c>
       <c r="AG3" s="8">
-        <f t="shared" si="0"/>
         <v>-3941196.7213114752</v>
       </c>
       <c r="AH3" s="8">
-        <f t="shared" si="0"/>
         <v>-5685786.8852459015</v>
       </c>
       <c r="AI3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AJ3" s="8">
-        <f t="shared" ref="AJ3:AK3" si="1">(AJ2-AJ4)/($A4-$A2)*($A4-$A3)+AJ4</f>
         <v>-21117491.803278688</v>
       </c>
       <c r="AK3" s="8">
-        <f t="shared" si="1"/>
         <v>-3085459.0163934426</v>
       </c>
       <c r="AL3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AM3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN3" s="8">
-        <f t="shared" ref="AN3" si="2">(AN2-AN4)/($A4-$A2)*($A4-$A3)+AN4</f>
         <v>61606.557377049176</v>
       </c>
       <c r="AO3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AP3" s="8">
-        <f t="shared" ref="AP3:AR3" si="3">(AP2-AP4)/($A4-$A2)*($A4-$A3)+AP4</f>
         <v>-20853885.245901637</v>
       </c>
       <c r="AQ3" s="8">
-        <f t="shared" si="3"/>
         <v>-98983.606557377061</v>
       </c>
       <c r="AR3" s="8">
-        <f t="shared" si="3"/>
         <v>-20952868.852459017</v>
       </c>
       <c r="AS3" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AT3" s="8">
-        <f t="shared" ref="AT3" si="4">(AT2-AT4)/($A4-$A2)*($A4-$A3)+AT4</f>
         <v>-20952868.852459017</v>
       </c>
     </row>
@@ -1224,149 +1065,138 @@
         <v>44012</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="W4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Y4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Z4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AA4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AC4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AD4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AE4" s="8">
-        <f t="shared" ref="AE4:AH4" si="5">(AE2-AE6)/($A6-$A2)*($A6-$A4)+AE6</f>
         <v>-6153448.0874316944</v>
       </c>
       <c r="AF4" s="8">
-        <f t="shared" si="5"/>
         <v>-5835945.3551912569</v>
       </c>
       <c r="AG4" s="8">
-        <f t="shared" si="5"/>
         <v>-3637797.8142076503</v>
       </c>
       <c r="AH4" s="8">
-        <f t="shared" si="5"/>
         <v>-5606857.923497268</v>
       </c>
       <c r="AI4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AJ4" s="8">
-        <f t="shared" ref="AJ4:AK4" si="6">(AJ2-AJ6)/($A6-$A2)*($A6-$A4)+AJ6</f>
         <v>-21547327.868852459</v>
       </c>
       <c r="AK4" s="8">
-        <f t="shared" si="6"/>
         <v>-2045306.0109289617</v>
       </c>
       <c r="AL4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AM4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN4" s="8">
-        <f t="shared" ref="AN4" si="7">(AN2-AN6)/($A6-$A2)*($A6-$A4)+AN6</f>
         <v>239071.03825136612</v>
       </c>
       <c r="AO4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AP4" s="8">
-        <f t="shared" ref="AP4:AR4" si="8">(AP2-AP6)/($A6-$A2)*($A6-$A4)+AP6</f>
         <v>-21029590.163934425</v>
       </c>
       <c r="AQ4" s="8">
-        <f t="shared" si="8"/>
         <v>-115322.40437158471</v>
       </c>
       <c r="AR4" s="8">
-        <f t="shared" si="8"/>
         <v>-21144912.56830601</v>
       </c>
       <c r="AS4" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AT4" s="8">
-        <f t="shared" ref="AT4" si="9">(AT2-AT6)/($A6-$A2)*($A6-$A4)+AT6</f>
         <v>-21144912.56830601</v>
       </c>
     </row>
@@ -1375,149 +1205,138 @@
         <v>44104</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Q5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Y5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Z5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AA5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AB5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AC5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AD5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AE5" s="8">
-        <f t="shared" ref="AE5:AH5" si="10">(AE4-AE6)/($A6-$A4)*($A6-$A5)+AE6</f>
         <v>-7078224.0437158477</v>
       </c>
       <c r="AF5" s="8">
-        <f t="shared" si="10"/>
         <v>-5564972.6775956284</v>
       </c>
       <c r="AG5" s="8">
-        <f t="shared" si="10"/>
         <v>-3334398.9071038254</v>
       </c>
       <c r="AH5" s="8">
-        <f t="shared" si="10"/>
         <v>-5527928.9617486335</v>
       </c>
       <c r="AI5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AJ5" s="8">
-        <f t="shared" ref="AJ5:AK5" si="11">(AJ4-AJ6)/($A6-$A4)*($A6-$A5)+AJ6</f>
         <v>-21977163.934426229</v>
       </c>
       <c r="AK5" s="8">
-        <f t="shared" si="11"/>
         <v>-1005153.0054644808</v>
       </c>
       <c r="AL5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AM5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN5" s="8">
-        <f t="shared" ref="AN5" si="12">(AN4-AN6)/($A6-$A4)*($A6-$A5)+AN6</f>
         <v>416535.51912568306</v>
       </c>
       <c r="AO5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AP5" s="8">
-        <f t="shared" ref="AP5:AR5" si="13">(AP4-AP6)/($A6-$A4)*($A6-$A5)+AP6</f>
         <v>-21205295.081967212</v>
       </c>
       <c r="AQ5" s="8">
-        <f t="shared" si="13"/>
         <v>-131661.20218579235</v>
       </c>
       <c r="AR5" s="8">
-        <f t="shared" si="13"/>
         <v>-21336956.284153007</v>
       </c>
       <c r="AS5" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AT5" s="8">
-        <f t="shared" ref="AT5" si="14">(AT4-AT6)/($A6-$A4)*($A6-$A5)+AT6</f>
         <v>-21336956.284153007</v>
       </c>
     </row>
@@ -1529,7 +1348,7 @@
         <v>17267000</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D6" s="7">
         <v>4000</v>
@@ -1559,10 +1378,10 @@
         <v>125085000</v>
       </c>
       <c r="M6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="N6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O6" s="7">
         <v>362000</v>
@@ -1589,16 +1408,16 @@
         <v>171906000</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="X6" s="7">
         <v>61253000</v>
       </c>
       <c r="Y6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Z6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AA6" s="7">
         <v>-117288000</v>
@@ -1607,10 +1426,10 @@
         <v>54618000</v>
       </c>
       <c r="AC6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AD6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AE6" s="7">
         <v>-8003000</v>
@@ -1625,7 +1444,7 @@
         <v>-5449000</v>
       </c>
       <c r="AI6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AJ6" s="7">
         <v>-22407000</v>
@@ -1634,16 +1453,16 @@
         <v>35000</v>
       </c>
       <c r="AL6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AM6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN6" s="7">
         <v>594000</v>
       </c>
       <c r="AO6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AP6" s="7">
         <v>-21381000</v>
@@ -1655,7 +1474,7 @@
         <v>-21529000</v>
       </c>
       <c r="AS6" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AT6" s="7">
         <v>-21529000</v>
@@ -1666,170 +1485,138 @@
         <v>44285</v>
       </c>
       <c r="B7" s="8">
-        <f>(B6-B8)/($A8-$A6)*($A8-$A7)+B8</f>
         <v>15137339.726027397</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D7" s="8">
-        <f t="shared" ref="D7:AT7" si="15">(D6-D8)/($A8-$A6)*($A8-$A7)+D8</f>
         <v>294652.05479452055</v>
       </c>
       <c r="E7" s="8">
-        <f t="shared" si="15"/>
         <v>1240895.8904109588</v>
       </c>
       <c r="F7" s="8">
-        <f t="shared" si="15"/>
         <v>16672887.671232877</v>
       </c>
       <c r="G7" s="8">
-        <f t="shared" si="15"/>
         <v>34300936.98630137</v>
       </c>
       <c r="H7" s="8">
-        <f t="shared" si="15"/>
         <v>1734550.6849315069</v>
       </c>
       <c r="I7" s="8">
-        <f t="shared" si="15"/>
         <v>27746687.671232879</v>
       </c>
       <c r="J7" s="8">
-        <f t="shared" si="15"/>
         <v>53471972.602739729</v>
       </c>
       <c r="K7" s="8">
-        <f t="shared" si="15"/>
         <v>3782624.6575342468</v>
       </c>
       <c r="L7" s="8">
-        <f t="shared" si="15"/>
         <v>121034402.73972602</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O7" s="8">
-        <f t="shared" si="15"/>
         <v>513909.58904109587</v>
       </c>
       <c r="P7" s="8">
-        <f t="shared" si="15"/>
         <v>572041.09589041094</v>
       </c>
       <c r="Q7" s="8">
-        <f t="shared" si="15"/>
         <v>7666704.1095890412</v>
       </c>
       <c r="R7" s="8">
-        <f t="shared" si="15"/>
         <v>168495964.38356164</v>
       </c>
       <c r="S7" s="8">
-        <f t="shared" si="15"/>
         <v>1291295.8904109588</v>
       </c>
       <c r="T7" s="8">
-        <f t="shared" si="15"/>
         <v>1000000</v>
       </c>
       <c r="U7" s="8">
-        <f t="shared" si="15"/>
         <v>649490.41095890407</v>
       </c>
       <c r="V7" s="8">
-        <f t="shared" si="15"/>
         <v>200543030.13698629</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="X7" s="8">
-        <f t="shared" si="15"/>
         <v>69840402.739726022</v>
       </c>
       <c r="Y7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Z7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AA7" s="8">
-        <f t="shared" si="15"/>
         <v>-152266219.1780822</v>
       </c>
       <c r="AB7" s="8">
-        <f t="shared" si="15"/>
         <v>53471972.602739729</v>
       </c>
       <c r="AC7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AD7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AE7" s="8">
-        <f t="shared" si="15"/>
         <v>-14985720.547945205</v>
       </c>
       <c r="AF7" s="8">
-        <f t="shared" si="15"/>
         <v>-6352734.2465753425</v>
       </c>
       <c r="AG7" s="8">
-        <f t="shared" si="15"/>
         <v>-4907802.7397260275</v>
       </c>
       <c r="AH7" s="8">
-        <f t="shared" si="15"/>
         <v>-7534526.0273972601</v>
       </c>
       <c r="AI7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AJ7" s="8">
-        <f t="shared" si="15"/>
         <v>-33679032.87671233</v>
       </c>
       <c r="AK7" s="8">
-        <f t="shared" si="15"/>
         <v>-2348005.4794520545</v>
       </c>
       <c r="AL7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AM7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN7" s="8">
-        <f t="shared" si="15"/>
         <v>709821.91780821909</v>
       </c>
       <c r="AO7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AP7" s="8">
-        <f t="shared" si="15"/>
         <v>-39706709.589041099</v>
       </c>
       <c r="AQ7" s="8">
-        <f t="shared" si="15"/>
         <v>-55342.465753424665</v>
       </c>
       <c r="AR7" s="8">
-        <f t="shared" si="15"/>
         <v>-39762052.05479452</v>
       </c>
       <c r="AS7" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AT7" s="8">
-        <f t="shared" si="15"/>
         <v>-39783021.91780822</v>
       </c>
     </row>
@@ -1838,170 +1625,138 @@
         <v>44377</v>
       </c>
       <c r="B8" s="8">
-        <f>(B6-B10)/($A10-$A6)*($A10-$A8)+B10</f>
         <v>12935893.15068493</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D8" s="8">
-        <f t="shared" ref="D8:AT8" si="16">(D6-D10)/($A10-$A6)*($A10-$A8)+D10</f>
         <v>595101.36986301374</v>
       </c>
       <c r="E8" s="8">
-        <f t="shared" si="16"/>
         <v>1725597.2602739725</v>
       </c>
       <c r="F8" s="8">
-        <f t="shared" si="16"/>
         <v>15256591.780821918</v>
       </c>
       <c r="G8" s="8">
-        <f t="shared" si="16"/>
         <v>33710624.657534249</v>
       </c>
       <c r="H8" s="8">
-        <f t="shared" si="16"/>
         <v>2141367.1232876712</v>
       </c>
       <c r="I8" s="8">
-        <f t="shared" si="16"/>
         <v>18620791.780821919</v>
       </c>
       <c r="J8" s="8">
-        <f t="shared" si="16"/>
         <v>52287315.06849315</v>
       </c>
       <c r="K8" s="8">
-        <f t="shared" si="16"/>
         <v>4738416.4383561648</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" si="16"/>
         <v>116847268.49315068</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="N8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O8" s="8">
-        <f t="shared" si="16"/>
         <v>670939.72602739721</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" si="16"/>
         <v>693027.39726027404</v>
       </c>
       <c r="Q8" s="8">
-        <f t="shared" si="16"/>
         <v>12922802.739726027</v>
       </c>
       <c r="R8" s="8">
-        <f t="shared" si="16"/>
         <v>206902309.58904111</v>
       </c>
       <c r="S8" s="8">
-        <f t="shared" si="16"/>
         <v>1555197.2602739725</v>
       </c>
       <c r="T8" s="8">
-        <f t="shared" si="16"/>
         <v>1000000</v>
       </c>
       <c r="U8" s="8">
-        <f t="shared" si="16"/>
         <v>1283660.2739726028</v>
       </c>
       <c r="V8" s="8">
-        <f t="shared" si="16"/>
         <v>230145353.42465752</v>
       </c>
       <c r="W8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="X8" s="8">
-        <f t="shared" si="16"/>
         <v>78717268.493150681</v>
       </c>
       <c r="Y8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Z8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AA8" s="8">
-        <f t="shared" si="16"/>
         <v>-188423479.4520548</v>
       </c>
       <c r="AB8" s="8">
-        <f t="shared" si="16"/>
         <v>52287315.06849315</v>
       </c>
       <c r="AC8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AD8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AE8" s="8">
-        <f t="shared" si="16"/>
         <v>-22203813.698630136</v>
       </c>
       <c r="AF8" s="8">
-        <f t="shared" si="16"/>
         <v>-7447156.1643835623</v>
       </c>
       <c r="AG8" s="8">
-        <f t="shared" si="16"/>
         <v>-6847868.493150685</v>
       </c>
       <c r="AH8" s="8">
-        <f t="shared" si="16"/>
         <v>-9690350.6849315055</v>
       </c>
       <c r="AI8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AJ8" s="8">
-        <f t="shared" si="16"/>
         <v>-45331021.91780822</v>
       </c>
       <c r="AK8" s="8">
-        <f t="shared" si="16"/>
         <v>-4811336.98630137</v>
       </c>
       <c r="AL8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AM8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN8" s="8">
-        <f t="shared" si="16"/>
         <v>829547.94520547939</v>
       </c>
       <c r="AO8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AP8" s="8">
-        <f t="shared" si="16"/>
         <v>-58650139.726027399</v>
       </c>
       <c r="AQ8" s="8">
-        <f t="shared" si="16"/>
         <v>40438.356164383556</v>
       </c>
       <c r="AR8" s="8">
-        <f t="shared" si="16"/>
         <v>-58609701.369863011</v>
       </c>
       <c r="AS8" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AT8" s="8">
-        <f t="shared" si="16"/>
         <v>-58652347.94520548</v>
       </c>
     </row>
@@ -2010,170 +1765,138 @@
         <v>44469</v>
       </c>
       <c r="B9" s="8">
-        <f>(B8-B10)/($A10-$A8)*($A10-$A9)+B10</f>
         <v>10734446.575342465</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" ref="D9:AT9" si="17">(D8-D10)/($A10-$A8)*($A10-$A9)+D10</f>
         <v>895550.68493150687</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" si="17"/>
         <v>2210298.6301369863</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" si="17"/>
         <v>13840295.89041096</v>
       </c>
       <c r="G9" s="8">
-        <f t="shared" si="17"/>
         <v>33120312.328767125</v>
       </c>
       <c r="H9" s="8">
-        <f t="shared" si="17"/>
         <v>2548183.5616438356</v>
       </c>
       <c r="I9" s="8">
-        <f t="shared" si="17"/>
         <v>9494895.8904109597</v>
       </c>
       <c r="J9" s="8">
-        <f t="shared" si="17"/>
         <v>51102657.534246579</v>
       </c>
       <c r="K9" s="8">
-        <f t="shared" si="17"/>
         <v>5694208.2191780824</v>
       </c>
       <c r="L9" s="8">
-        <f t="shared" si="17"/>
         <v>112660134.24657534</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O9" s="8">
-        <f t="shared" si="17"/>
         <v>827969.8630136986</v>
       </c>
       <c r="P9" s="8">
-        <f t="shared" si="17"/>
         <v>814013.69863013702</v>
       </c>
       <c r="Q9" s="8">
-        <f t="shared" si="17"/>
         <v>18178901.369863015</v>
       </c>
       <c r="R9" s="8">
-        <f t="shared" si="17"/>
         <v>245308654.79452056</v>
       </c>
       <c r="S9" s="8">
-        <f t="shared" si="17"/>
         <v>1819098.6301369863</v>
       </c>
       <c r="T9" s="8">
-        <f t="shared" si="17"/>
         <v>1000000</v>
       </c>
       <c r="U9" s="8">
-        <f t="shared" si="17"/>
         <v>1917830.1369863013</v>
       </c>
       <c r="V9" s="8">
-        <f t="shared" si="17"/>
         <v>259747676.71232876</v>
       </c>
       <c r="W9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="X9" s="8">
-        <f t="shared" si="17"/>
         <v>87594134.246575341</v>
       </c>
       <c r="Y9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Z9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AA9" s="8">
-        <f t="shared" si="17"/>
         <v>-224580739.7260274</v>
       </c>
       <c r="AB9" s="8">
-        <f t="shared" si="17"/>
         <v>51102657.534246579</v>
       </c>
       <c r="AC9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AD9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AE9" s="8">
-        <f t="shared" si="17"/>
         <v>-29421906.84931507</v>
       </c>
       <c r="AF9" s="8">
-        <f t="shared" si="17"/>
         <v>-8541578.0821917802</v>
       </c>
       <c r="AG9" s="8">
-        <f t="shared" si="17"/>
         <v>-8787934.2465753425</v>
       </c>
       <c r="AH9" s="8">
-        <f t="shared" si="17"/>
         <v>-11846175.342465753</v>
       </c>
       <c r="AI9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AJ9" s="8">
-        <f t="shared" si="17"/>
         <v>-56983010.95890411</v>
       </c>
       <c r="AK9" s="8">
-        <f t="shared" si="17"/>
         <v>-7274668.493150685</v>
       </c>
       <c r="AL9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AM9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN9" s="8">
-        <f t="shared" si="17"/>
         <v>949273.9726027397</v>
       </c>
       <c r="AO9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AP9" s="8">
-        <f t="shared" si="17"/>
         <v>-77593569.8630137</v>
       </c>
       <c r="AQ9" s="8">
-        <f t="shared" si="17"/>
         <v>136219.17808219179</v>
       </c>
       <c r="AR9" s="8">
-        <f t="shared" si="17"/>
         <v>-77457350.684931502</v>
       </c>
       <c r="AS9" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AT9" s="8">
-        <f t="shared" si="17"/>
         <v>-77521673.97260274</v>
       </c>
     </row>
@@ -2185,7 +1908,7 @@
         <v>8533000</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D10" s="7">
         <v>1196000</v>
@@ -2218,7 +1941,7 @@
         <v>143237000</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O10" s="7">
         <v>985000</v>
@@ -2322,179 +2045,138 @@
         <v>44650</v>
       </c>
       <c r="B11" s="8">
-        <f>(B10-B12)/($A12-$A10)*($A12-$A11)+B12</f>
         <v>25112602.739726026</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" ref="D11:AL11" si="18">(D10-D12)/($A12-$A10)*($A12-$A11)+D12</f>
         <v>1242816.4383561644</v>
       </c>
       <c r="E11" s="8">
-        <f t="shared" si="18"/>
         <v>2817649.3150684931</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="18"/>
         <v>29203791.780821919</v>
       </c>
       <c r="G11" s="8">
-        <f t="shared" si="18"/>
         <v>36297504.10958904</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" si="18"/>
         <v>4226846.5753424652</v>
       </c>
       <c r="I11" s="8">
-        <f t="shared" si="18"/>
         <v>1854934.2465753423</v>
       </c>
       <c r="J11" s="8">
-        <f t="shared" si="18"/>
         <v>72823186.301369861</v>
       </c>
       <c r="K11" s="8">
-        <f t="shared" si="18"/>
         <v>7430273.9726027399</v>
       </c>
       <c r="L11" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M11" s="8">
-        <f t="shared" si="18"/>
         <v>110343087.67123288</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O11" s="8">
-        <f t="shared" si="18"/>
         <v>1275408.2191780824</v>
       </c>
       <c r="P11" s="8">
-        <f t="shared" si="18"/>
         <v>1180298.6301369863</v>
       </c>
       <c r="Q11" s="8">
-        <f t="shared" si="18"/>
         <v>19285405.479452055</v>
       </c>
       <c r="R11" s="8">
-        <f t="shared" si="18"/>
         <v>221867802.73972601</v>
       </c>
       <c r="S11" s="8">
-        <f t="shared" si="18"/>
         <v>3053465.7534246575</v>
       </c>
       <c r="T11" s="8">
-        <f t="shared" si="18"/>
         <v>1000000</v>
       </c>
       <c r="U11" s="8">
-        <f t="shared" si="18"/>
         <v>2057013.6986301369</v>
       </c>
       <c r="V11" s="8">
-        <f t="shared" si="18"/>
         <v>227978282.19178084</v>
       </c>
       <c r="W11" s="8">
-        <f t="shared" si="18"/>
         <v>-131363263.01369864</v>
       </c>
       <c r="X11" s="8">
-        <f t="shared" si="18"/>
         <v>155346816.43835616</v>
       </c>
       <c r="Y11" s="8">
-        <f t="shared" si="18"/>
         <v>-141106.84931506851</v>
       </c>
       <c r="Z11" s="8">
-        <f t="shared" si="18"/>
         <v>-195108380.8219178</v>
       </c>
       <c r="AA11" s="8">
-        <f t="shared" si="18"/>
         <v>-171265934.24657536</v>
       </c>
       <c r="AB11" s="8">
-        <f t="shared" si="18"/>
         <v>72823186.301369861</v>
       </c>
       <c r="AC11" s="8">
-        <f t="shared" si="18"/>
         <v>4677369.8630136987</v>
       </c>
       <c r="AD11" s="8">
-        <f t="shared" si="18"/>
         <v>-2219320.5479452056</v>
       </c>
       <c r="AE11" s="8">
-        <f t="shared" si="18"/>
         <v>-36774353.424657539</v>
       </c>
       <c r="AF11" s="8">
-        <f t="shared" si="18"/>
         <v>-10469673.97260274</v>
       </c>
       <c r="AG11" s="8">
-        <f t="shared" si="18"/>
         <v>-11605320.547945205</v>
       </c>
       <c r="AH11" s="8">
-        <f t="shared" si="18"/>
         <v>-17664654.794520549</v>
       </c>
       <c r="AI11" s="8">
-        <f t="shared" si="18"/>
         <v>-78733323.287671238</v>
       </c>
       <c r="AJ11" s="8">
-        <f t="shared" si="18"/>
         <v>-74055953.424657539</v>
       </c>
       <c r="AK11" s="8">
-        <f t="shared" si="18"/>
         <v>-7522509.5890410952</v>
       </c>
       <c r="AL11" s="8">
-        <f t="shared" si="18"/>
         <v>27816402.739726026</v>
       </c>
       <c r="AM11" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN11" s="8">
-        <f t="shared" ref="AN11:AT11" si="19">(AN10-AN12)/($A12-$A10)*($A12-$A11)+AN12</f>
         <v>1086312.3287671234</v>
       </c>
       <c r="AO11" s="8">
-        <f t="shared" si="19"/>
         <v>-6761208.2191780806</v>
       </c>
       <c r="AP11" s="8">
-        <f t="shared" si="19"/>
         <v>-80817161.643835619</v>
       </c>
       <c r="AQ11" s="8">
-        <f t="shared" si="19"/>
         <v>-939630.13698630151</v>
       </c>
       <c r="AR11" s="8">
-        <f t="shared" si="19"/>
         <v>-81756791.780821919</v>
       </c>
       <c r="AS11" s="8">
-        <f t="shared" si="19"/>
         <v>-120136.98630136985</v>
       </c>
       <c r="AT11" s="8">
-        <f t="shared" si="19"/>
         <v>-81876928.767123297</v>
       </c>
     </row>
@@ -2503,179 +2185,138 @@
         <v>44742</v>
       </c>
       <c r="B12" s="8">
-        <f>(B10-B14)/($A14-$A10)*($A14-$A12)+B14</f>
         <v>42251068.493150681</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D12" s="8">
-        <f t="shared" ref="D12:K12" si="20">(D10-D14)/($A14-$A10)*($A14-$A12)+D14</f>
         <v>1291210.9589041097</v>
       </c>
       <c r="E12" s="8">
-        <f t="shared" si="20"/>
         <v>2944432.8767123288</v>
       </c>
       <c r="F12" s="8">
-        <f t="shared" si="20"/>
         <v>46549194.520547949</v>
       </c>
       <c r="G12" s="8">
-        <f t="shared" si="20"/>
         <v>40192002.739726029</v>
       </c>
       <c r="H12" s="8">
-        <f t="shared" si="20"/>
         <v>5541564.3835616438</v>
       </c>
       <c r="I12" s="8">
-        <f t="shared" si="20"/>
         <v>3390956.1643835614</v>
       </c>
       <c r="J12" s="8">
-        <f t="shared" si="20"/>
         <v>96500457.534246564</v>
       </c>
       <c r="K12" s="8">
-        <f t="shared" si="20"/>
         <v>8236849.3150684927</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M12" s="8">
-        <f t="shared" ref="M12" si="21">(M10-M14)/($A14-$A10)*($A14-$A12)+M14</f>
         <v>76340391.780821919</v>
       </c>
       <c r="N12" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O12" s="8">
-        <f t="shared" ref="O12:AT12" si="22">(O10-O14)/($A14-$A10)*($A14-$A12)+O14</f>
         <v>1575605.4794520549</v>
       </c>
       <c r="P12" s="8">
-        <f t="shared" si="22"/>
         <v>1433865.7534246575</v>
       </c>
       <c r="Q12" s="8">
-        <f t="shared" si="22"/>
         <v>14995936.98630137</v>
       </c>
       <c r="R12" s="8">
-        <f t="shared" si="22"/>
         <v>157935868.49315068</v>
       </c>
       <c r="S12" s="8">
-        <f t="shared" si="22"/>
         <v>4056643.8356164386</v>
       </c>
       <c r="T12" s="8">
-        <f t="shared" si="22"/>
         <v>1000000</v>
       </c>
       <c r="U12" s="8">
-        <f t="shared" si="22"/>
         <v>1545342.4657534244</v>
       </c>
       <c r="V12" s="8">
-        <f t="shared" si="22"/>
         <v>164537854.79452056</v>
       </c>
       <c r="W12" s="8">
-        <f t="shared" si="22"/>
         <v>-90443175.342465758</v>
       </c>
       <c r="X12" s="8">
-        <f t="shared" si="22"/>
         <v>216207210.95890409</v>
       </c>
       <c r="Y12" s="8">
-        <f t="shared" si="22"/>
         <v>-198071.23287671234</v>
       </c>
       <c r="Z12" s="8">
-        <f t="shared" si="22"/>
         <v>-204343920.5479452</v>
       </c>
       <c r="AA12" s="8">
-        <f t="shared" si="22"/>
         <v>-78777956.16438356</v>
       </c>
       <c r="AB12" s="8">
-        <f t="shared" si="22"/>
         <v>96500457.534246564</v>
       </c>
       <c r="AC12" s="8">
-        <f t="shared" si="22"/>
         <v>5122246.5753424661</v>
       </c>
       <c r="AD12" s="8">
-        <f t="shared" si="22"/>
         <v>-2574213.6986301369</v>
       </c>
       <c r="AE12" s="8">
-        <f t="shared" si="22"/>
         <v>-36913235.616438359</v>
       </c>
       <c r="AF12" s="8">
-        <f t="shared" si="22"/>
         <v>-11331449.315068493</v>
       </c>
       <c r="AG12" s="8">
-        <f t="shared" si="22"/>
         <v>-12512213.698630137</v>
       </c>
       <c r="AH12" s="8">
-        <f t="shared" si="22"/>
         <v>-21450769.8630137</v>
       </c>
       <c r="AI12" s="8">
-        <f t="shared" si="22"/>
         <v>-84781882.19178082</v>
       </c>
       <c r="AJ12" s="8">
-        <f t="shared" si="22"/>
         <v>-79659635.616438359</v>
       </c>
       <c r="AK12" s="8">
-        <f t="shared" si="22"/>
         <v>-5232339.7260273974</v>
       </c>
       <c r="AL12" s="8">
-        <f t="shared" si="22"/>
         <v>37981268.493150681</v>
       </c>
       <c r="AM12" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN12" s="8">
-        <f t="shared" si="22"/>
         <v>1104208.2191780822</v>
       </c>
       <c r="AO12" s="8">
-        <f t="shared" si="22"/>
         <v>15092194.520547949</v>
       </c>
       <c r="AP12" s="8">
-        <f t="shared" si="22"/>
         <v>-64567441.095890418</v>
       </c>
       <c r="AQ12" s="8">
-        <f t="shared" si="22"/>
         <v>-2150753.4246575343</v>
       </c>
       <c r="AR12" s="8">
-        <f t="shared" si="22"/>
         <v>-66718194.520547949</v>
       </c>
       <c r="AS12" s="8">
-        <f t="shared" si="22"/>
         <v>-155424.65753424657</v>
       </c>
       <c r="AT12" s="8">
-        <f t="shared" si="22"/>
         <v>-66873619.178082198</v>
       </c>
     </row>
@@ -2684,179 +2325,138 @@
         <v>44834</v>
       </c>
       <c r="B13" s="8">
-        <f>(B12-B14)/($A14-$A12)*($A14-$A13)+B14</f>
         <v>59389534.246575341</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D13" s="8">
-        <f t="shared" ref="D13:AL13" si="23">(D12-D14)/($A14-$A12)*($A14-$A13)+D14</f>
         <v>1339605.4794520549</v>
       </c>
       <c r="E13" s="8">
-        <f t="shared" si="23"/>
         <v>3071216.4383561644</v>
       </c>
       <c r="F13" s="8">
-        <f t="shared" si="23"/>
         <v>63894597.260273978</v>
       </c>
       <c r="G13" s="8">
-        <f t="shared" si="23"/>
         <v>44086501.369863011</v>
       </c>
       <c r="H13" s="8">
-        <f t="shared" si="23"/>
         <v>6856282.1917808224</v>
       </c>
       <c r="I13" s="8">
-        <f t="shared" si="23"/>
         <v>4926978.0821917802</v>
       </c>
       <c r="J13" s="8">
-        <f t="shared" si="23"/>
         <v>120177728.76712328</v>
       </c>
       <c r="K13" s="8">
-        <f t="shared" si="23"/>
         <v>9043424.6575342473</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M13" s="8">
-        <f t="shared" si="23"/>
         <v>42337695.89041096</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="O13" s="8">
-        <f t="shared" si="23"/>
         <v>1875802.7397260275</v>
       </c>
       <c r="P13" s="8">
-        <f t="shared" si="23"/>
         <v>1687432.8767123288</v>
       </c>
       <c r="Q13" s="8">
-        <f t="shared" si="23"/>
         <v>10706468.493150685</v>
       </c>
       <c r="R13" s="8">
-        <f t="shared" si="23"/>
         <v>94003934.246575341</v>
       </c>
       <c r="S13" s="8">
-        <f t="shared" si="23"/>
         <v>5059821.9178082198</v>
       </c>
       <c r="T13" s="8">
-        <f t="shared" si="23"/>
         <v>1000000</v>
       </c>
       <c r="U13" s="8">
-        <f t="shared" si="23"/>
         <v>1033671.2328767122</v>
       </c>
       <c r="V13" s="8">
-        <f t="shared" si="23"/>
         <v>101097427.39726028</v>
       </c>
       <c r="W13" s="8">
-        <f t="shared" si="23"/>
         <v>-49523087.671232879</v>
       </c>
       <c r="X13" s="8">
-        <f t="shared" si="23"/>
         <v>277067605.47945201</v>
       </c>
       <c r="Y13" s="8">
-        <f t="shared" si="23"/>
         <v>-255035.61643835617</v>
       </c>
       <c r="Z13" s="8">
-        <f t="shared" si="23"/>
         <v>-213579460.2739726</v>
       </c>
       <c r="AA13" s="8">
-        <f t="shared" si="23"/>
         <v>13710021.91780822</v>
       </c>
       <c r="AB13" s="8">
-        <f t="shared" si="23"/>
         <v>120177728.76712328</v>
       </c>
       <c r="AC13" s="8">
-        <f t="shared" si="23"/>
         <v>5567123.2876712326</v>
       </c>
       <c r="AD13" s="8">
-        <f t="shared" si="23"/>
         <v>-2929106.8493150687</v>
       </c>
       <c r="AE13" s="8">
-        <f t="shared" si="23"/>
         <v>-37052117.80821918</v>
       </c>
       <c r="AF13" s="8">
-        <f t="shared" si="23"/>
         <v>-12193224.657534247</v>
       </c>
       <c r="AG13" s="8">
-        <f t="shared" si="23"/>
         <v>-13419106.84931507</v>
       </c>
       <c r="AH13" s="8">
-        <f t="shared" si="23"/>
         <v>-25236884.93150685</v>
       </c>
       <c r="AI13" s="8">
-        <f t="shared" si="23"/>
         <v>-90830441.095890403</v>
       </c>
       <c r="AJ13" s="8">
-        <f t="shared" si="23"/>
         <v>-85263317.80821918</v>
       </c>
       <c r="AK13" s="8">
-        <f t="shared" si="23"/>
         <v>-2942169.8630136987</v>
       </c>
       <c r="AL13" s="8">
-        <f t="shared" si="23"/>
         <v>48146134.246575341</v>
       </c>
       <c r="AM13" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN13" s="8">
-        <f t="shared" ref="AN13:AT13" si="24">(AN12-AN14)/($A14-$A12)*($A14-$A13)+AN14</f>
         <v>1122104.1095890412</v>
       </c>
       <c r="AO13" s="8">
-        <f t="shared" si="24"/>
         <v>36945597.260273978</v>
       </c>
       <c r="AP13" s="8">
-        <f t="shared" si="24"/>
         <v>-48317720.547945209</v>
       </c>
       <c r="AQ13" s="8">
-        <f t="shared" si="24"/>
         <v>-3361876.7123287674</v>
       </c>
       <c r="AR13" s="8">
-        <f t="shared" si="24"/>
         <v>-51679597.260273978</v>
       </c>
       <c r="AS13" s="8">
-        <f t="shared" si="24"/>
         <v>-190712.32876712328</v>
       </c>
       <c r="AT13" s="8">
-        <f t="shared" si="24"/>
         <v>-51870309.589041099</v>
       </c>
     </row>
@@ -2895,7 +2495,7 @@
         <v>9850000</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M14" s="7">
         <v>8335000</v>
@@ -2976,7 +2576,7 @@
         <v>58311000</v>
       </c>
       <c r="AM14" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN14" s="7">
         <v>1140000</v>
@@ -3005,180 +2605,138 @@
         <v>45015</v>
       </c>
       <c r="B15" s="8">
-        <f t="shared" ref="B15" si="25">(B14-B16)/($A16-$A14)*($A16-$A15)+B16</f>
         <v>63592032.87671233</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D15" s="8">
-        <f t="shared" ref="D15:K15" si="26">(D14-D16)/($A16-$A14)*($A16-$A15)+D16</f>
         <v>1269252.0547945206</v>
       </c>
       <c r="E15" s="8">
-        <f t="shared" si="26"/>
         <v>2948068.493150685</v>
       </c>
       <c r="F15" s="8">
-        <f t="shared" si="26"/>
         <v>67904630.1369863</v>
       </c>
       <c r="G15" s="8">
-        <f t="shared" si="26"/>
         <v>46310482.19178082</v>
       </c>
       <c r="H15" s="8">
-        <f t="shared" si="26"/>
         <v>6957673.9726027399</v>
       </c>
       <c r="I15" s="8">
-        <f t="shared" si="26"/>
         <v>6229893.1506849313</v>
       </c>
       <c r="J15" s="8">
-        <f t="shared" si="26"/>
         <v>127402679.4520548</v>
       </c>
       <c r="K15" s="8">
-        <f t="shared" si="26"/>
         <v>9383054.7945205476</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M15" s="8">
-        <f t="shared" ref="M15:AL15" si="27">(M14-M16)/($A16-$A14)*($A16-$A15)+M16</f>
         <v>6984150.6849315073</v>
       </c>
       <c r="N15" s="8">
-        <f t="shared" si="27"/>
         <v>1125257.5342465753</v>
       </c>
       <c r="O15" s="8">
-        <f t="shared" si="27"/>
         <v>2167953.4246575343</v>
       </c>
       <c r="P15" s="8">
-        <f t="shared" si="27"/>
         <v>2376734.2465753425</v>
       </c>
       <c r="Q15" s="8">
-        <f t="shared" si="27"/>
         <v>5918356.1643835614</v>
       </c>
       <c r="R15" s="8">
-        <f t="shared" si="27"/>
         <v>27955506.84931507</v>
       </c>
       <c r="S15" s="8">
-        <f t="shared" si="27"/>
         <v>5020846.5753424652</v>
       </c>
       <c r="T15" s="8">
-        <f t="shared" si="27"/>
         <v>1000000</v>
       </c>
       <c r="U15" s="8">
-        <f t="shared" si="27"/>
         <v>522975.34246575343</v>
       </c>
       <c r="V15" s="8">
-        <f t="shared" si="27"/>
         <v>34499328.767123289</v>
       </c>
       <c r="W15" s="8">
-        <f t="shared" si="27"/>
         <v>-8603000</v>
       </c>
       <c r="X15" s="8">
-        <f t="shared" si="27"/>
         <v>339443682.19178081</v>
       </c>
       <c r="Y15" s="8">
-        <f t="shared" si="27"/>
         <v>-243969.86301369863</v>
       </c>
       <c r="Z15" s="8">
-        <f t="shared" si="27"/>
         <v>-237693361.6438356</v>
       </c>
       <c r="AA15" s="8">
-        <f t="shared" si="27"/>
         <v>92903350.684931517</v>
       </c>
       <c r="AB15" s="8">
-        <f t="shared" si="27"/>
         <v>127402679.4520548</v>
       </c>
       <c r="AC15" s="8">
-        <f t="shared" si="27"/>
         <v>7002460.2739726026</v>
       </c>
       <c r="AD15" s="8">
-        <f t="shared" si="27"/>
         <v>-3716076.7123287669</v>
       </c>
       <c r="AE15" s="8">
-        <f t="shared" si="27"/>
         <v>-33852646.575342469</v>
       </c>
       <c r="AF15" s="8">
-        <f t="shared" si="27"/>
         <v>-12470038.356164385</v>
       </c>
       <c r="AG15" s="8">
-        <f t="shared" si="27"/>
         <v>-15040438.356164385</v>
       </c>
       <c r="AH15" s="8">
-        <f t="shared" si="27"/>
         <v>-27556572.602739725</v>
       </c>
       <c r="AI15" s="8">
-        <f t="shared" si="27"/>
         <v>-92635772.602739722</v>
       </c>
       <c r="AJ15" s="8">
-        <f t="shared" si="27"/>
         <v>-85633312.328767121</v>
       </c>
       <c r="AK15" s="8">
-        <f t="shared" si="27"/>
         <v>-73134.246575342375</v>
       </c>
       <c r="AL15" s="8">
-        <f t="shared" si="27"/>
         <v>45671293.15068493</v>
       </c>
       <c r="AM15" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN15" s="8">
-        <f t="shared" ref="AN15:AT15" si="28">(AN14-AN16)/($A16-$A14)*($A16-$A15)+AN16</f>
         <v>3122627.3972602738</v>
       </c>
       <c r="AO15" s="8">
-        <f t="shared" si="28"/>
         <v>48720786.301369861</v>
       </c>
       <c r="AP15" s="8">
-        <f t="shared" si="28"/>
         <v>-36912526.02739726</v>
       </c>
       <c r="AQ15" s="8">
-        <f t="shared" si="28"/>
         <v>-5672454.7945205476</v>
       </c>
       <c r="AR15" s="8">
-        <f t="shared" si="28"/>
         <v>-42584980.82191781</v>
       </c>
       <c r="AS15" s="8">
-        <f t="shared" si="28"/>
         <v>-102863.01369863015</v>
       </c>
       <c r="AT15" s="8">
-        <f t="shared" si="28"/>
         <v>-42687843.83561644</v>
       </c>
     </row>
@@ -3187,180 +2745,138 @@
         <v>45107</v>
       </c>
       <c r="B16" s="8">
-        <f t="shared" ref="B16" si="29">(B14-B18)/($A18-$A14)*($A18-$A16)+B18</f>
         <v>50220021.91780822</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D16" s="8">
-        <f t="shared" ref="D16:K16" si="30">(D14-D18)/($A18-$A14)*($A18-$A16)+D18</f>
         <v>1146501.3698630137</v>
       </c>
       <c r="E16" s="8">
-        <f t="shared" si="30"/>
         <v>2689712.3287671232</v>
       </c>
       <c r="F16" s="8">
-        <f t="shared" si="30"/>
         <v>54119753.424657539</v>
       </c>
       <c r="G16" s="8">
-        <f t="shared" si="30"/>
         <v>44583654.794520549</v>
       </c>
       <c r="H16" s="8">
-        <f t="shared" si="30"/>
         <v>5703449.3150684927</v>
       </c>
       <c r="I16" s="8">
-        <f t="shared" si="30"/>
         <v>5988928.7671232875</v>
       </c>
       <c r="J16" s="8">
-        <f t="shared" si="30"/>
         <v>110395786.30136986</v>
       </c>
       <c r="K16" s="8">
-        <f t="shared" si="30"/>
         <v>8900369.8630136978</v>
       </c>
       <c r="L16" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M16" s="8">
-        <f t="shared" ref="M16:AL16" si="31">(M14-M18)/($A18-$A14)*($A18-$A16)+M18</f>
         <v>5587767.1232876712</v>
       </c>
       <c r="N16" s="8">
-        <f t="shared" si="31"/>
         <v>889838.35616438359</v>
       </c>
       <c r="O16" s="8">
-        <f t="shared" si="31"/>
         <v>2159635.6164383562</v>
       </c>
       <c r="P16" s="8">
-        <f t="shared" si="31"/>
         <v>2827156.1643835618</v>
       </c>
       <c r="Q16" s="8">
-        <f t="shared" si="31"/>
         <v>5402904.1095890412</v>
       </c>
       <c r="R16" s="8">
-        <f t="shared" si="31"/>
         <v>25767671.232876711</v>
       </c>
       <c r="S16" s="8">
-        <f t="shared" si="31"/>
         <v>3943564.3835616438</v>
       </c>
       <c r="T16" s="8">
-        <f t="shared" si="31"/>
         <v>1000000</v>
       </c>
       <c r="U16" s="8">
-        <f t="shared" si="31"/>
         <v>523983.56164383562</v>
       </c>
       <c r="V16" s="8">
-        <f t="shared" si="31"/>
         <v>31235219.17808219</v>
       </c>
       <c r="W16" s="8">
-        <f t="shared" si="31"/>
         <v>-8603000</v>
       </c>
       <c r="X16" s="8">
-        <f t="shared" si="31"/>
         <v>341010454.79452056</v>
       </c>
       <c r="Y16" s="8">
-        <f t="shared" si="31"/>
         <v>-173646.57534246575</v>
       </c>
       <c r="Z16" s="8">
-        <f t="shared" si="31"/>
         <v>-253073241.0958904</v>
       </c>
       <c r="AA16" s="8">
-        <f t="shared" si="31"/>
         <v>79160567.123287678</v>
       </c>
       <c r="AB16" s="8">
-        <f t="shared" si="31"/>
         <v>110395786.30136986</v>
       </c>
       <c r="AC16" s="8">
-        <f t="shared" si="31"/>
         <v>8026306.8493150687</v>
       </c>
       <c r="AD16" s="8">
-        <f t="shared" si="31"/>
         <v>-4162717.8082191781</v>
       </c>
       <c r="AE16" s="8">
-        <f t="shared" si="31"/>
         <v>-30401764.383561645</v>
       </c>
       <c r="AF16" s="8">
-        <f t="shared" si="31"/>
         <v>-11865358.90410959</v>
       </c>
       <c r="AG16" s="8">
-        <f t="shared" si="31"/>
         <v>-15778958.90410959</v>
       </c>
       <c r="AH16" s="8">
-        <f t="shared" si="31"/>
         <v>-26040715.06849315</v>
       </c>
       <c r="AI16" s="8">
-        <f t="shared" si="31"/>
         <v>-88249515.068493158</v>
       </c>
       <c r="AJ16" s="8">
-        <f t="shared" si="31"/>
         <v>-80223208.219178081</v>
       </c>
       <c r="AK16" s="8">
-        <f t="shared" si="31"/>
         <v>525243.83561643842</v>
       </c>
       <c r="AL16" s="8">
-        <f t="shared" si="31"/>
         <v>32605528.767123289</v>
       </c>
       <c r="AM16" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN16" s="8">
-        <f t="shared" ref="AN16:AT16" si="32">(AN14-AN18)/($A18-$A14)*($A18-$A16)+AN18</f>
         <v>5172084.9315068498</v>
       </c>
       <c r="AO16" s="8">
-        <f t="shared" si="32"/>
         <v>38302857.534246579</v>
       </c>
       <c r="AP16" s="8">
-        <f t="shared" si="32"/>
         <v>-41920350.684931509</v>
       </c>
       <c r="AQ16" s="8">
-        <f t="shared" si="32"/>
         <v>-6808969.8630136987</v>
       </c>
       <c r="AR16" s="8">
-        <f t="shared" si="32"/>
         <v>-48729320.547945209</v>
       </c>
       <c r="AS16" s="8">
-        <f t="shared" si="32"/>
         <v>24424.657534246566</v>
       </c>
       <c r="AT16" s="8">
-        <f t="shared" si="32"/>
         <v>-48704895.89041096</v>
       </c>
     </row>
@@ -3369,180 +2885,138 @@
         <v>45199</v>
       </c>
       <c r="B17" s="8">
-        <f t="shared" ref="B17" si="33">(B16-B18)/($A18-$A16)*($A18-$A17)+B18</f>
         <v>36848010.95890411</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D17" s="8">
-        <f t="shared" ref="D17:K17" si="34">(D16-D18)/($A18-$A16)*($A18-$A17)+D18</f>
         <v>1023750.6849315069</v>
       </c>
       <c r="E17" s="8">
-        <f t="shared" si="34"/>
         <v>2431356.1643835618</v>
       </c>
       <c r="F17" s="8">
-        <f t="shared" si="34"/>
         <v>40334876.712328769</v>
       </c>
       <c r="G17" s="8">
-        <f t="shared" si="34"/>
         <v>42856827.397260278</v>
       </c>
       <c r="H17" s="8">
-        <f t="shared" si="34"/>
         <v>4449224.6575342463</v>
       </c>
       <c r="I17" s="8">
-        <f t="shared" si="34"/>
         <v>5747964.3835616438</v>
       </c>
       <c r="J17" s="8">
-        <f t="shared" si="34"/>
         <v>93388893.150684923</v>
       </c>
       <c r="K17" s="8">
-        <f t="shared" si="34"/>
         <v>8417684.9315068498</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M17" s="8">
-        <f t="shared" ref="M17:AL17" si="35">(M16-M18)/($A18-$A16)*($A18-$A17)+M18</f>
         <v>4191383.5616438356</v>
       </c>
       <c r="N17" s="8">
-        <f t="shared" si="35"/>
         <v>654419.17808219185</v>
       </c>
       <c r="O17" s="8">
-        <f t="shared" si="35"/>
         <v>2151317.8082191781</v>
       </c>
       <c r="P17" s="8">
-        <f t="shared" si="35"/>
         <v>3277578.0821917811</v>
       </c>
       <c r="Q17" s="8">
-        <f t="shared" si="35"/>
         <v>4887452.0547945211</v>
       </c>
       <c r="R17" s="8">
-        <f t="shared" si="35"/>
         <v>23579835.616438355</v>
       </c>
       <c r="S17" s="8">
-        <f t="shared" si="35"/>
         <v>2866282.1917808219</v>
       </c>
       <c r="T17" s="8">
-        <f t="shared" si="35"/>
         <v>1000000</v>
       </c>
       <c r="U17" s="8">
-        <f t="shared" si="35"/>
         <v>524991.78082191781</v>
       </c>
       <c r="V17" s="8">
-        <f t="shared" si="35"/>
         <v>27971109.589041095</v>
       </c>
       <c r="W17" s="8">
-        <f t="shared" si="35"/>
         <v>-8603000</v>
       </c>
       <c r="X17" s="8">
-        <f t="shared" si="35"/>
         <v>342577227.39726031</v>
       </c>
       <c r="Y17" s="8">
-        <f t="shared" si="35"/>
         <v>-103323.28767123287</v>
       </c>
       <c r="Z17" s="8">
-        <f t="shared" si="35"/>
         <v>-268453120.5479452</v>
       </c>
       <c r="AA17" s="8">
-        <f t="shared" si="35"/>
         <v>65417783.561643839</v>
       </c>
       <c r="AB17" s="8">
-        <f t="shared" si="35"/>
         <v>93388893.150684923</v>
       </c>
       <c r="AC17" s="8">
-        <f t="shared" si="35"/>
         <v>9050153.4246575348</v>
       </c>
       <c r="AD17" s="8">
-        <f t="shared" si="35"/>
         <v>-4609358.9041095888</v>
       </c>
       <c r="AE17" s="8">
-        <f t="shared" si="35"/>
         <v>-26950882.19178082</v>
       </c>
       <c r="AF17" s="8">
-        <f t="shared" si="35"/>
         <v>-11260679.452054795</v>
       </c>
       <c r="AG17" s="8">
-        <f t="shared" si="35"/>
         <v>-16517479.452054795</v>
       </c>
       <c r="AH17" s="8">
-        <f t="shared" si="35"/>
         <v>-24524857.534246575</v>
       </c>
       <c r="AI17" s="8">
-        <f t="shared" si="35"/>
         <v>-83863257.534246579</v>
       </c>
       <c r="AJ17" s="8">
-        <f t="shared" si="35"/>
         <v>-74813104.10958904</v>
       </c>
       <c r="AK17" s="8">
-        <f t="shared" si="35"/>
         <v>1123621.9178082193</v>
       </c>
       <c r="AL17" s="8">
-        <f t="shared" si="35"/>
         <v>19539764.383561645</v>
       </c>
       <c r="AM17" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN17" s="8">
-        <f t="shared" ref="AN17:AT17" si="36">(AN16-AN18)/($A18-$A16)*($A18-$A17)+AN18</f>
         <v>7221542.4657534249</v>
       </c>
       <c r="AO17" s="8">
-        <f t="shared" si="36"/>
         <v>27884928.767123289</v>
       </c>
       <c r="AP17" s="8">
-        <f t="shared" si="36"/>
         <v>-46928175.342465758</v>
       </c>
       <c r="AQ17" s="8">
-        <f t="shared" si="36"/>
         <v>-7945484.9315068498</v>
       </c>
       <c r="AR17" s="8">
-        <f t="shared" si="36"/>
         <v>-54873660.273972601</v>
       </c>
       <c r="AS17" s="8">
-        <f t="shared" si="36"/>
         <v>151712.32876712328</v>
       </c>
       <c r="AT17" s="8">
-        <f t="shared" si="36"/>
         <v>-54721947.94520548</v>
       </c>
     </row>
@@ -3554,7 +3028,7 @@
         <v>23476000</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="D18" s="7">
         <v>901000</v>
@@ -3581,7 +3055,7 @@
         <v>7935000</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="M18" s="7">
         <v>2795000</v>
@@ -3662,7 +3136,7 @@
         <v>6474000</v>
       </c>
       <c r="AM18" s="7" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="AN18" s="7">
         <v>9271000</v>

</xml_diff>

<commit_message>
[ADD] change '-' to '0' in satellogic empty columns
</commit_message>
<xml_diff>
--- a/financial_data/satellogic.xlsx
+++ b/financial_data/satellogic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holly\space_econometrics\financial_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C638CF28-776C-4091-AC37-177B3032AB03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D89456-5C37-46D9-A624-21A87E8D99C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{84ACD714-4695-47C3-B1A3-494310BA187C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Revenue</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>Foreign currency translation gain (loss), netoftax</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t>Restricted cash</t>
@@ -599,7 +596,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28921E86-815C-4D28-B61B-DA9A063C903A}">
   <dimension ref="A1:AT18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="AS2" sqref="AS2:AS9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -644,73 +643,73 @@
   <sheetData>
     <row r="1" spans="1:46" s="5" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="T1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>4</v>
@@ -722,43 +721,43 @@
         <v>5</v>
       </c>
       <c r="AA1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="AI1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="AJ1" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AK1" s="4" t="s">
         <v>12</v>
       </c>
       <c r="AL1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AM1" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="AM1" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="AN1" s="3" t="s">
         <v>1</v>
@@ -767,111 +766,111 @@
         <v>13</v>
       </c>
       <c r="AP1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" s="4" t="s">
+      <c r="AR1" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="AS1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="AT1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>43830</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD2" s="6" t="s">
-        <v>15</v>
+      <c r="B2" s="6">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6">
+        <v>0</v>
+      </c>
+      <c r="J2" s="6">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>0</v>
+      </c>
+      <c r="R2" s="6">
+        <v>0</v>
+      </c>
+      <c r="S2" s="6">
+        <v>0</v>
+      </c>
+      <c r="T2" s="6">
+        <v>0</v>
+      </c>
+      <c r="U2" s="6">
+        <v>0</v>
+      </c>
+      <c r="V2" s="6">
+        <v>0</v>
+      </c>
+      <c r="W2" s="6">
+        <v>0</v>
+      </c>
+      <c r="X2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>0</v>
       </c>
       <c r="AE2" s="6">
         <v>-4324000</v>
@@ -885,8 +884,8 @@
       <c r="AH2" s="6">
         <v>-5763000</v>
       </c>
-      <c r="AI2" s="6" t="s">
-        <v>15</v>
+      <c r="AI2" s="6">
+        <v>0</v>
       </c>
       <c r="AJ2" s="6">
         <v>-20697000</v>
@@ -894,17 +893,17 @@
       <c r="AK2" s="6">
         <v>-4103000</v>
       </c>
-      <c r="AL2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM2" s="6" t="s">
-        <v>15</v>
+      <c r="AL2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="6">
+        <v>0</v>
       </c>
       <c r="AN2" s="6">
         <v>-112000</v>
       </c>
-      <c r="AO2" s="6" t="s">
-        <v>15</v>
+      <c r="AO2" s="6">
+        <v>0</v>
       </c>
       <c r="AP2" s="6">
         <v>-20682000</v>
@@ -915,8 +914,8 @@
       <c r="AR2" s="6">
         <v>-20765000</v>
       </c>
-      <c r="AS2" s="6" t="s">
-        <v>15</v>
+      <c r="AS2" s="6">
+        <v>0</v>
       </c>
       <c r="AT2" s="6">
         <v>-20765000</v>
@@ -926,92 +925,92 @@
       <c r="A3" s="7">
         <v>43920</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="W3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="X3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>15</v>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <v>0</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>0</v>
+      </c>
+      <c r="R3" s="6">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6">
+        <v>0</v>
+      </c>
+      <c r="T3" s="6">
+        <v>0</v>
+      </c>
+      <c r="U3" s="6">
+        <v>0</v>
+      </c>
+      <c r="V3" s="6">
+        <v>0</v>
+      </c>
+      <c r="W3" s="6">
+        <v>0</v>
+      </c>
+      <c r="X3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="6">
+        <v>0</v>
       </c>
       <c r="AE3" s="6">
         <v>-5228672.1311475411</v>
@@ -1025,8 +1024,8 @@
       <c r="AH3" s="6">
         <v>-5685786.8852459015</v>
       </c>
-      <c r="AI3" s="6" t="s">
-        <v>15</v>
+      <c r="AI3" s="6">
+        <v>0</v>
       </c>
       <c r="AJ3" s="6">
         <v>-21117491.803278688</v>
@@ -1034,17 +1033,17 @@
       <c r="AK3" s="6">
         <v>-3085459.0163934426</v>
       </c>
-      <c r="AL3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM3" s="6" t="s">
-        <v>15</v>
+      <c r="AL3" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="6">
+        <v>0</v>
       </c>
       <c r="AN3" s="6">
         <v>61606.557377049176</v>
       </c>
-      <c r="AO3" s="6" t="s">
-        <v>15</v>
+      <c r="AO3" s="6">
+        <v>0</v>
       </c>
       <c r="AP3" s="6">
         <v>-20853885.245901637</v>
@@ -1055,8 +1054,8 @@
       <c r="AR3" s="6">
         <v>-20952868.852459017</v>
       </c>
-      <c r="AS3" s="6" t="s">
-        <v>15</v>
+      <c r="AS3" s="6">
+        <v>0</v>
       </c>
       <c r="AT3" s="6">
         <v>-20952868.852459017</v>
@@ -1066,92 +1065,92 @@
       <c r="A4" s="7">
         <v>44012</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="U4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="V4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="W4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="X4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD4" s="6" t="s">
-        <v>15</v>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6">
+        <v>0</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <v>0</v>
+      </c>
+      <c r="O4" s="6">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+      <c r="T4" s="6">
+        <v>0</v>
+      </c>
+      <c r="U4" s="6">
+        <v>0</v>
+      </c>
+      <c r="V4" s="6">
+        <v>0</v>
+      </c>
+      <c r="W4" s="6">
+        <v>0</v>
+      </c>
+      <c r="X4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="6">
+        <v>0</v>
       </c>
       <c r="AE4" s="6">
         <v>-6153448.0874316944</v>
@@ -1165,8 +1164,8 @@
       <c r="AH4" s="6">
         <v>-5606857.923497268</v>
       </c>
-      <c r="AI4" s="6" t="s">
-        <v>15</v>
+      <c r="AI4" s="6">
+        <v>0</v>
       </c>
       <c r="AJ4" s="6">
         <v>-21547327.868852459</v>
@@ -1174,17 +1173,17 @@
       <c r="AK4" s="6">
         <v>-2045306.0109289617</v>
       </c>
-      <c r="AL4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM4" s="6" t="s">
-        <v>15</v>
+      <c r="AL4" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="6">
+        <v>0</v>
       </c>
       <c r="AN4" s="6">
         <v>239071.03825136612</v>
       </c>
-      <c r="AO4" s="6" t="s">
-        <v>15</v>
+      <c r="AO4" s="6">
+        <v>0</v>
       </c>
       <c r="AP4" s="6">
         <v>-21029590.163934425</v>
@@ -1195,8 +1194,8 @@
       <c r="AR4" s="6">
         <v>-21144912.56830601</v>
       </c>
-      <c r="AS4" s="6" t="s">
-        <v>15</v>
+      <c r="AS4" s="6">
+        <v>0</v>
       </c>
       <c r="AT4" s="6">
         <v>-21144912.56830601</v>
@@ -1206,92 +1205,92 @@
       <c r="A5" s="7">
         <v>44104</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="U5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="V5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="W5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="X5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Y5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AB5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AC5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD5" s="6" t="s">
-        <v>15</v>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6">
+        <v>0</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+      <c r="R5" s="6">
+        <v>0</v>
+      </c>
+      <c r="S5" s="6">
+        <v>0</v>
+      </c>
+      <c r="T5" s="6">
+        <v>0</v>
+      </c>
+      <c r="U5" s="6">
+        <v>0</v>
+      </c>
+      <c r="V5" s="6">
+        <v>0</v>
+      </c>
+      <c r="W5" s="6">
+        <v>0</v>
+      </c>
+      <c r="X5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="6">
+        <v>0</v>
       </c>
       <c r="AE5" s="6">
         <v>-7078224.0437158477</v>
@@ -1305,8 +1304,8 @@
       <c r="AH5" s="6">
         <v>-5527928.9617486335</v>
       </c>
-      <c r="AI5" s="6" t="s">
-        <v>15</v>
+      <c r="AI5" s="6">
+        <v>0</v>
       </c>
       <c r="AJ5" s="6">
         <v>-21977163.934426229</v>
@@ -1314,17 +1313,17 @@
       <c r="AK5" s="6">
         <v>-1005153.0054644808</v>
       </c>
-      <c r="AL5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM5" s="6" t="s">
-        <v>15</v>
+      <c r="AL5" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="6">
+        <v>0</v>
       </c>
       <c r="AN5" s="6">
         <v>416535.51912568306</v>
       </c>
-      <c r="AO5" s="6" t="s">
-        <v>15</v>
+      <c r="AO5" s="6">
+        <v>0</v>
       </c>
       <c r="AP5" s="6">
         <v>-21205295.081967212</v>
@@ -1335,8 +1334,8 @@
       <c r="AR5" s="6">
         <v>-21336956.284153007</v>
       </c>
-      <c r="AS5" s="6" t="s">
-        <v>15</v>
+      <c r="AS5" s="6">
+        <v>0</v>
       </c>
       <c r="AT5" s="6">
         <v>-21336956.284153007</v>
@@ -1349,8 +1348,8 @@
       <c r="B6" s="6">
         <v>17267000</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>15</v>
+      <c r="C6" s="6">
+        <v>0</v>
       </c>
       <c r="D6" s="6">
         <v>4000</v>
@@ -1379,11 +1378,11 @@
       <c r="L6" s="6">
         <v>125085000</v>
       </c>
-      <c r="M6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>15</v>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0</v>
       </c>
       <c r="O6" s="6">
         <v>362000</v>
@@ -1409,17 +1408,17 @@
       <c r="V6" s="6">
         <v>171906000</v>
       </c>
-      <c r="W6" s="6" t="s">
-        <v>15</v>
+      <c r="W6" s="6">
+        <v>0</v>
       </c>
       <c r="X6" s="6">
         <v>61253000</v>
       </c>
-      <c r="Y6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z6" s="6" t="s">
-        <v>15</v>
+      <c r="Y6" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="6">
+        <v>0</v>
       </c>
       <c r="AA6" s="6">
         <v>-117288000</v>
@@ -1427,11 +1426,11 @@
       <c r="AB6" s="6">
         <v>54618000</v>
       </c>
-      <c r="AC6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD6" s="6" t="s">
-        <v>15</v>
+      <c r="AC6" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="6">
+        <v>0</v>
       </c>
       <c r="AE6" s="6">
         <v>-8003000</v>
@@ -1445,8 +1444,8 @@
       <c r="AH6" s="6">
         <v>-5449000</v>
       </c>
-      <c r="AI6" s="6" t="s">
-        <v>15</v>
+      <c r="AI6" s="6">
+        <v>0</v>
       </c>
       <c r="AJ6" s="6">
         <v>-22407000</v>
@@ -1454,17 +1453,17 @@
       <c r="AK6" s="6">
         <v>35000</v>
       </c>
-      <c r="AL6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM6" s="6" t="s">
-        <v>15</v>
+      <c r="AL6" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="6">
+        <v>0</v>
       </c>
       <c r="AN6" s="6">
         <v>594000</v>
       </c>
-      <c r="AO6" s="6" t="s">
-        <v>15</v>
+      <c r="AO6" s="6">
+        <v>0</v>
       </c>
       <c r="AP6" s="6">
         <v>-21381000</v>
@@ -1475,8 +1474,8 @@
       <c r="AR6" s="6">
         <v>-21529000</v>
       </c>
-      <c r="AS6" s="6" t="s">
-        <v>15</v>
+      <c r="AS6" s="6">
+        <v>0</v>
       </c>
       <c r="AT6" s="6">
         <v>-21529000</v>
@@ -1489,8 +1488,8 @@
       <c r="B7" s="6">
         <v>15137339.726027397</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>15</v>
+      <c r="C7" s="6">
+        <v>0</v>
       </c>
       <c r="D7" s="6">
         <v>294652.05479452055</v>
@@ -1519,11 +1518,11 @@
       <c r="L7" s="6">
         <v>121034402.73972602</v>
       </c>
-      <c r="M7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>15</v>
+      <c r="M7" s="6">
+        <v>0</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0</v>
       </c>
       <c r="O7" s="6">
         <v>513909.58904109587</v>
@@ -1549,17 +1548,17 @@
       <c r="V7" s="6">
         <v>200543030.13698629</v>
       </c>
-      <c r="W7" s="6" t="s">
-        <v>15</v>
+      <c r="W7" s="6">
+        <v>0</v>
       </c>
       <c r="X7" s="6">
         <v>69840402.739726022</v>
       </c>
-      <c r="Y7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z7" s="6" t="s">
-        <v>15</v>
+      <c r="Y7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="6">
+        <v>0</v>
       </c>
       <c r="AA7" s="6">
         <v>-152266219.1780822</v>
@@ -1567,11 +1566,11 @@
       <c r="AB7" s="6">
         <v>53471972.602739729</v>
       </c>
-      <c r="AC7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD7" s="6" t="s">
-        <v>15</v>
+      <c r="AC7" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="6">
+        <v>0</v>
       </c>
       <c r="AE7" s="6">
         <v>-14985720.547945205</v>
@@ -1585,8 +1584,8 @@
       <c r="AH7" s="6">
         <v>-7534526.0273972601</v>
       </c>
-      <c r="AI7" s="6" t="s">
-        <v>15</v>
+      <c r="AI7" s="6">
+        <v>0</v>
       </c>
       <c r="AJ7" s="6">
         <v>-33679032.87671233</v>
@@ -1594,17 +1593,17 @@
       <c r="AK7" s="6">
         <v>-2348005.4794520545</v>
       </c>
-      <c r="AL7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM7" s="6" t="s">
-        <v>15</v>
+      <c r="AL7" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="6">
+        <v>0</v>
       </c>
       <c r="AN7" s="6">
         <v>709821.91780821909</v>
       </c>
-      <c r="AO7" s="6" t="s">
-        <v>15</v>
+      <c r="AO7" s="6">
+        <v>0</v>
       </c>
       <c r="AP7" s="6">
         <v>-39706709.589041099</v>
@@ -1615,8 +1614,8 @@
       <c r="AR7" s="6">
         <v>-39762052.05479452</v>
       </c>
-      <c r="AS7" s="6" t="s">
-        <v>15</v>
+      <c r="AS7" s="6">
+        <v>0</v>
       </c>
       <c r="AT7" s="6">
         <v>-39783021.91780822</v>
@@ -1629,8 +1628,8 @@
       <c r="B8" s="6">
         <v>12935893.15068493</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>15</v>
+      <c r="C8" s="6">
+        <v>0</v>
       </c>
       <c r="D8" s="6">
         <v>595101.36986301374</v>
@@ -1659,11 +1658,11 @@
       <c r="L8" s="6">
         <v>116847268.49315068</v>
       </c>
-      <c r="M8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>15</v>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0</v>
       </c>
       <c r="O8" s="6">
         <v>670939.72602739721</v>
@@ -1689,17 +1688,17 @@
       <c r="V8" s="6">
         <v>230145353.42465752</v>
       </c>
-      <c r="W8" s="6" t="s">
-        <v>15</v>
+      <c r="W8" s="6">
+        <v>0</v>
       </c>
       <c r="X8" s="6">
         <v>78717268.493150681</v>
       </c>
-      <c r="Y8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z8" s="6" t="s">
-        <v>15</v>
+      <c r="Y8" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="6">
+        <v>0</v>
       </c>
       <c r="AA8" s="6">
         <v>-188423479.4520548</v>
@@ -1707,11 +1706,11 @@
       <c r="AB8" s="6">
         <v>52287315.06849315</v>
       </c>
-      <c r="AC8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD8" s="6" t="s">
-        <v>15</v>
+      <c r="AC8" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="6">
+        <v>0</v>
       </c>
       <c r="AE8" s="6">
         <v>-22203813.698630136</v>
@@ -1725,8 +1724,8 @@
       <c r="AH8" s="6">
         <v>-9690350.6849315055</v>
       </c>
-      <c r="AI8" s="6" t="s">
-        <v>15</v>
+      <c r="AI8" s="6">
+        <v>0</v>
       </c>
       <c r="AJ8" s="6">
         <v>-45331021.91780822</v>
@@ -1734,17 +1733,17 @@
       <c r="AK8" s="6">
         <v>-4811336.98630137</v>
       </c>
-      <c r="AL8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM8" s="6" t="s">
-        <v>15</v>
+      <c r="AL8" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="6">
+        <v>0</v>
       </c>
       <c r="AN8" s="6">
         <v>829547.94520547939</v>
       </c>
-      <c r="AO8" s="6" t="s">
-        <v>15</v>
+      <c r="AO8" s="6">
+        <v>0</v>
       </c>
       <c r="AP8" s="6">
         <v>-58650139.726027399</v>
@@ -1755,8 +1754,8 @@
       <c r="AR8" s="6">
         <v>-58609701.369863011</v>
       </c>
-      <c r="AS8" s="6" t="s">
-        <v>15</v>
+      <c r="AS8" s="6">
+        <v>0</v>
       </c>
       <c r="AT8" s="6">
         <v>-58652347.94520548</v>
@@ -1769,8 +1768,8 @@
       <c r="B9" s="6">
         <v>10734446.575342465</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>15</v>
+      <c r="C9" s="6">
+        <v>0</v>
       </c>
       <c r="D9" s="6">
         <v>895550.68493150687</v>
@@ -1799,11 +1798,11 @@
       <c r="L9" s="6">
         <v>112660134.24657534</v>
       </c>
-      <c r="M9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>15</v>
+      <c r="M9" s="6">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6">
+        <v>0</v>
       </c>
       <c r="O9" s="6">
         <v>827969.8630136986</v>
@@ -1829,17 +1828,17 @@
       <c r="V9" s="6">
         <v>259747676.71232876</v>
       </c>
-      <c r="W9" s="6" t="s">
-        <v>15</v>
+      <c r="W9" s="6">
+        <v>0</v>
       </c>
       <c r="X9" s="6">
         <v>87594134.246575341</v>
       </c>
-      <c r="Y9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="Z9" s="6" t="s">
-        <v>15</v>
+      <c r="Y9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="6">
+        <v>0</v>
       </c>
       <c r="AA9" s="6">
         <v>-224580739.7260274</v>
@@ -1847,11 +1846,11 @@
       <c r="AB9" s="6">
         <v>51102657.534246579</v>
       </c>
-      <c r="AC9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD9" s="6" t="s">
-        <v>15</v>
+      <c r="AC9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="6">
+        <v>0</v>
       </c>
       <c r="AE9" s="6">
         <v>-29421906.84931507</v>
@@ -1865,8 +1864,8 @@
       <c r="AH9" s="6">
         <v>-11846175.342465753</v>
       </c>
-      <c r="AI9" s="6" t="s">
-        <v>15</v>
+      <c r="AI9" s="6">
+        <v>0</v>
       </c>
       <c r="AJ9" s="6">
         <v>-56983010.95890411</v>
@@ -1874,17 +1873,17 @@
       <c r="AK9" s="6">
         <v>-7274668.493150685</v>
       </c>
-      <c r="AL9" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="AM9" s="6" t="s">
-        <v>15</v>
+      <c r="AL9" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="6">
+        <v>0</v>
       </c>
       <c r="AN9" s="6">
         <v>949273.9726027397</v>
       </c>
-      <c r="AO9" s="6" t="s">
-        <v>15</v>
+      <c r="AO9" s="6">
+        <v>0</v>
       </c>
       <c r="AP9" s="6">
         <v>-77593569.8630137</v>
@@ -1895,8 +1894,8 @@
       <c r="AR9" s="6">
         <v>-77457350.684931502</v>
       </c>
-      <c r="AS9" s="6" t="s">
-        <v>15</v>
+      <c r="AS9" s="6">
+        <v>0</v>
       </c>
       <c r="AT9" s="6">
         <v>-77521673.97260274</v>
@@ -1909,8 +1908,8 @@
       <c r="B10" s="6">
         <v>8533000</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>15</v>
+      <c r="C10" s="6">
+        <v>0</v>
       </c>
       <c r="D10" s="6">
         <v>1196000</v>
@@ -1942,8 +1941,8 @@
       <c r="M10" s="6">
         <v>143237000</v>
       </c>
-      <c r="N10" s="6" t="s">
-        <v>15</v>
+      <c r="N10" s="6">
+        <v>0</v>
       </c>
       <c r="O10" s="6">
         <v>985000</v>
@@ -2049,8 +2048,8 @@
       <c r="B11" s="6">
         <v>25112602.739726026</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>15</v>
+      <c r="C11" s="6">
+        <v>0</v>
       </c>
       <c r="D11" s="6">
         <v>1242816.4383561644</v>
@@ -2076,14 +2075,14 @@
       <c r="K11" s="6">
         <v>7430273.9726027399</v>
       </c>
-      <c r="L11" s="6" t="s">
-        <v>15</v>
+      <c r="L11" s="6">
+        <v>0</v>
       </c>
       <c r="M11" s="6">
         <v>110343087.67123288</v>
       </c>
-      <c r="N11" s="6" t="s">
-        <v>15</v>
+      <c r="N11" s="6">
+        <v>0</v>
       </c>
       <c r="O11" s="6">
         <v>1275408.2191780824</v>
@@ -2157,8 +2156,8 @@
       <c r="AL11" s="6">
         <v>27816402.739726026</v>
       </c>
-      <c r="AM11" s="6" t="s">
-        <v>15</v>
+      <c r="AM11" s="6">
+        <v>0</v>
       </c>
       <c r="AN11" s="6">
         <v>1086312.3287671234</v>
@@ -2189,8 +2188,8 @@
       <c r="B12" s="6">
         <v>42251068.493150681</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>15</v>
+      <c r="C12" s="6">
+        <v>0</v>
       </c>
       <c r="D12" s="6">
         <v>1291210.9589041097</v>
@@ -2216,14 +2215,14 @@
       <c r="K12" s="6">
         <v>8236849.3150684927</v>
       </c>
-      <c r="L12" s="6" t="s">
-        <v>15</v>
+      <c r="L12" s="6">
+        <v>0</v>
       </c>
       <c r="M12" s="6">
         <v>76340391.780821919</v>
       </c>
-      <c r="N12" s="6" t="s">
-        <v>15</v>
+      <c r="N12" s="6">
+        <v>0</v>
       </c>
       <c r="O12" s="6">
         <v>1575605.4794520549</v>
@@ -2297,8 +2296,8 @@
       <c r="AL12" s="6">
         <v>37981268.493150681</v>
       </c>
-      <c r="AM12" s="6" t="s">
-        <v>15</v>
+      <c r="AM12" s="6">
+        <v>0</v>
       </c>
       <c r="AN12" s="6">
         <v>1104208.2191780822</v>
@@ -2329,8 +2328,8 @@
       <c r="B13" s="6">
         <v>59389534.246575341</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>15</v>
+      <c r="C13" s="6">
+        <v>0</v>
       </c>
       <c r="D13" s="6">
         <v>1339605.4794520549</v>
@@ -2356,14 +2355,14 @@
       <c r="K13" s="6">
         <v>9043424.6575342473</v>
       </c>
-      <c r="L13" s="6" t="s">
-        <v>15</v>
+      <c r="L13" s="6">
+        <v>0</v>
       </c>
       <c r="M13" s="6">
         <v>42337695.89041096</v>
       </c>
-      <c r="N13" s="6" t="s">
-        <v>15</v>
+      <c r="N13" s="6">
+        <v>0</v>
       </c>
       <c r="O13" s="6">
         <v>1875802.7397260275</v>
@@ -2437,8 +2436,8 @@
       <c r="AL13" s="6">
         <v>48146134.246575341</v>
       </c>
-      <c r="AM13" s="6" t="s">
-        <v>15</v>
+      <c r="AM13" s="6">
+        <v>0</v>
       </c>
       <c r="AN13" s="6">
         <v>1122104.1095890412</v>
@@ -2496,8 +2495,8 @@
       <c r="K14" s="6">
         <v>9850000</v>
       </c>
-      <c r="L14" s="6" t="s">
-        <v>15</v>
+      <c r="L14" s="6">
+        <v>0</v>
       </c>
       <c r="M14" s="6">
         <v>8335000</v>
@@ -2577,8 +2576,8 @@
       <c r="AL14" s="6">
         <v>58311000</v>
       </c>
-      <c r="AM14" s="6" t="s">
-        <v>15</v>
+      <c r="AM14" s="6">
+        <v>0</v>
       </c>
       <c r="AN14" s="6">
         <v>1140000</v>
@@ -2609,8 +2608,8 @@
       <c r="B15" s="6">
         <v>63592032.87671233</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>15</v>
+      <c r="C15" s="6">
+        <v>0</v>
       </c>
       <c r="D15" s="6">
         <v>1269252.0547945206</v>
@@ -2636,8 +2635,8 @@
       <c r="K15" s="6">
         <v>9383054.7945205476</v>
       </c>
-      <c r="L15" s="6" t="s">
-        <v>15</v>
+      <c r="L15" s="6">
+        <v>0</v>
       </c>
       <c r="M15" s="6">
         <v>6984150.6849315073</v>
@@ -2717,8 +2716,8 @@
       <c r="AL15" s="6">
         <v>45671293.15068493</v>
       </c>
-      <c r="AM15" s="6" t="s">
-        <v>15</v>
+      <c r="AM15" s="6">
+        <v>0</v>
       </c>
       <c r="AN15" s="6">
         <v>3122627.3972602738</v>
@@ -2749,8 +2748,8 @@
       <c r="B16" s="6">
         <v>50220021.91780822</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>15</v>
+      <c r="C16" s="6">
+        <v>0</v>
       </c>
       <c r="D16" s="6">
         <v>1146501.3698630137</v>
@@ -2776,8 +2775,8 @@
       <c r="K16" s="6">
         <v>8900369.8630136978</v>
       </c>
-      <c r="L16" s="6" t="s">
-        <v>15</v>
+      <c r="L16" s="6">
+        <v>0</v>
       </c>
       <c r="M16" s="6">
         <v>5587767.1232876712</v>
@@ -2857,8 +2856,8 @@
       <c r="AL16" s="6">
         <v>32605528.767123289</v>
       </c>
-      <c r="AM16" s="6" t="s">
-        <v>15</v>
+      <c r="AM16" s="6">
+        <v>0</v>
       </c>
       <c r="AN16" s="6">
         <v>5172084.9315068498</v>
@@ -2889,8 +2888,8 @@
       <c r="B17" s="6">
         <v>36848010.95890411</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>15</v>
+      <c r="C17" s="6">
+        <v>0</v>
       </c>
       <c r="D17" s="6">
         <v>1023750.6849315069</v>
@@ -2916,8 +2915,8 @@
       <c r="K17" s="6">
         <v>8417684.9315068498</v>
       </c>
-      <c r="L17" s="6" t="s">
-        <v>15</v>
+      <c r="L17" s="6">
+        <v>0</v>
       </c>
       <c r="M17" s="6">
         <v>4191383.5616438356</v>
@@ -2997,8 +2996,8 @@
       <c r="AL17" s="6">
         <v>19539764.383561645</v>
       </c>
-      <c r="AM17" s="6" t="s">
-        <v>15</v>
+      <c r="AM17" s="6">
+        <v>0</v>
       </c>
       <c r="AN17" s="6">
         <v>7221542.4657534249</v>
@@ -3029,8 +3028,8 @@
       <c r="B18" s="6">
         <v>23476000</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>15</v>
+      <c r="C18" s="6">
+        <v>0</v>
       </c>
       <c r="D18" s="6">
         <v>901000</v>
@@ -3056,8 +3055,8 @@
       <c r="K18" s="6">
         <v>7935000</v>
       </c>
-      <c r="L18" s="6" t="s">
-        <v>15</v>
+      <c r="L18" s="6">
+        <v>0</v>
       </c>
       <c r="M18" s="6">
         <v>2795000</v>
@@ -3137,8 +3136,8 @@
       <c r="AL18" s="6">
         <v>6474000</v>
       </c>
-      <c r="AM18" s="6" t="s">
-        <v>15</v>
+      <c r="AM18" s="6">
+        <v>0</v>
       </c>
       <c r="AN18" s="6">
         <v>9271000</v>

</xml_diff>

<commit_message>
[MAJOR] add titles to ACF/PACF plots, plot num of sats and frac constellation, make heading titles for this consistent in data, add Kleos Space to all plots
</commit_message>
<xml_diff>
--- a/financial_data/satellogic.xlsx
+++ b/financial_data/satellogic.xlsx
@@ -1,212 +1,177 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\22028\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A268BA-6A7B-419D-927E-1647AB2B4A81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16410" yWindow="345" windowWidth="10605" windowHeight="15630" xr2:uid="{84ACD714-4695-47C3-B1A3-494310BA187C}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="consolidated" sheetId="3" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="consolidated"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
+    <t>Quarter</t>
+  </si>
+  <si>
+    <t>Total Launched Satellites</t>
+  </si>
+  <si>
+    <t>Cash and cash equivalents</t>
+  </si>
+  <si>
+    <t>Restricted cash</t>
+  </si>
+  <si>
+    <t>Accounts receivable</t>
+  </si>
+  <si>
+    <t>Prepaid expenses and other currentassets</t>
+  </si>
+  <si>
+    <t>Total Current Assets</t>
+  </si>
+  <si>
+    <t>Property and equipment,net</t>
+  </si>
+  <si>
+    <t>Operating lease right-of-use assets</t>
+  </si>
+  <si>
+    <t>Other non-current assets</t>
+  </si>
+  <si>
+    <t>Total Assets</t>
+  </si>
+  <si>
+    <t>Accounts payable</t>
+  </si>
+  <si>
+    <t>Debt</t>
+  </si>
+  <si>
+    <t>Warrant liabilities</t>
+  </si>
+  <si>
+    <t>Earnout liabilities</t>
+  </si>
+  <si>
+    <t>Operating lease liabilities (current liabilities)</t>
+  </si>
+  <si>
+    <t>Contract liabilities (current liabilities)</t>
+  </si>
+  <si>
+    <t>Accrued expenses and other liabilities</t>
+  </si>
+  <si>
+    <t>Total Current Liabilities</t>
+  </si>
+  <si>
+    <t>Operating lease liabilities</t>
+  </si>
+  <si>
+    <t>Contract liabilities</t>
+  </si>
+  <si>
+    <t>Other non-current liabilities</t>
+  </si>
+  <si>
+    <t>Total Liabilities</t>
+  </si>
+  <si>
+    <t>Treasury stock, at cost</t>
+  </si>
+  <si>
+    <t>Additional paid-in capital</t>
+  </si>
+  <si>
+    <t>Accumulated other comprehensive loss</t>
+  </si>
+  <si>
+    <t>Accumulated deficit</t>
+  </si>
+  <si>
+    <t>Total Equity</t>
+  </si>
+  <si>
+    <t>Liabilities and Equity</t>
+  </si>
+  <si>
     <t>Revenue</t>
   </si>
   <si>
+    <t>Cost of sales</t>
+  </si>
+  <si>
+    <t>General and administrative expenses</t>
+  </si>
+  <si>
+    <t>Research and development</t>
+  </si>
+  <si>
+    <t>Depreciation expense</t>
+  </si>
+  <si>
+    <t>Other operating expenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total costs and expenses </t>
+  </si>
+  <si>
+    <t>Total operating expenses</t>
+  </si>
+  <si>
+    <t>Finance income (expense), net</t>
+  </si>
+  <si>
+    <t>Change in fair value offinancial instrnments</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Loss on extinguishment of debt</t>
+  </si>
+  <si>
     <t>Other income, net</t>
   </si>
   <si>
-    <t>Cash and cash equivalents</t>
-  </si>
-  <si>
-    <t>Operating lease right-of-use assets</t>
-  </si>
-  <si>
-    <t>Additional paid-in capital</t>
-  </si>
-  <si>
-    <t>Accumulated deficit</t>
-  </si>
-  <si>
-    <t>Accrued expenses and other liabilities</t>
-  </si>
-  <si>
-    <t>Debt</t>
-  </si>
-  <si>
-    <t>Prepaid expenses and other currentassets</t>
-  </si>
-  <si>
-    <t>Operating lease liabilities</t>
-  </si>
-  <si>
-    <t>Accumulated other comprehensive loss</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total costs and expenses </t>
-  </si>
-  <si>
-    <t>Finance income (expense), net</t>
-  </si>
-  <si>
     <t>Total other income (expense), net</t>
   </si>
   <si>
+    <t>Loss before income tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Income tax (expense)  benefit </t>
+  </si>
+  <si>
+    <t>Net loss available to stockholders Other comprehensive loss</t>
+  </si>
+  <si>
     <t>Foreign currency translation gain (loss), netoftax</t>
   </si>
   <si>
-    <t>Restricted cash</t>
-  </si>
-  <si>
-    <t>Accounts receivable</t>
-  </si>
-  <si>
-    <t>Total Current Assets</t>
-  </si>
-  <si>
-    <t>Property and equipment,net</t>
-  </si>
-  <si>
-    <t>Other non-current assets</t>
-  </si>
-  <si>
-    <t>Total Assets</t>
-  </si>
-  <si>
-    <t>Accounts payable</t>
-  </si>
-  <si>
-    <t>Warrant liabilities</t>
-  </si>
-  <si>
-    <t>Earnout liabilities</t>
-  </si>
-  <si>
-    <t>Operating lease liabilities (current liabilities)</t>
-  </si>
-  <si>
-    <t>Contract liabilities (current liabilities)</t>
-  </si>
-  <si>
-    <t>Total Current Liabilities</t>
-  </si>
-  <si>
-    <t>Contract liabilities</t>
-  </si>
-  <si>
-    <t>Other non-current liabilities</t>
-  </si>
-  <si>
-    <t>Total Liabilities</t>
-  </si>
-  <si>
-    <t>Treasury stock, at cost</t>
-  </si>
-  <si>
-    <t>Total Equity</t>
-  </si>
-  <si>
-    <t>Liabilities and Equity</t>
-  </si>
-  <si>
-    <t>Cost of sales</t>
-  </si>
-  <si>
-    <t>General and administrative expenses</t>
-  </si>
-  <si>
-    <t>Research and development</t>
-  </si>
-  <si>
-    <t>Depreciation expense</t>
-  </si>
-  <si>
-    <t>Other operating expenses</t>
-  </si>
-  <si>
-    <t>Total operating expenses</t>
-  </si>
-  <si>
-    <t>Change in fair value offinancial instrnments</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Loss on extinguishment of debt</t>
-  </si>
-  <si>
-    <t>Loss before income tax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Income tax (expense)  benefit </t>
-  </si>
-  <si>
-    <t>Net loss available to stockholders Other comprehensive loss</t>
-  </si>
-  <si>
     <t>Net loss</t>
-  </si>
-  <si>
-    <t>Quarter</t>
-  </si>
-  <si>
-    <t>Total Launch Satellites</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
-    <numFmt numFmtId="26" formatCode="\$#,##0.00_);[Red]\(\$#,##0.00\)"/>
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="181" formatCode="0_);[Red]\(0\)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="$#,##0_);($#,##0)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -216,16 +181,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="游ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -236,7 +194,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -248,44 +213,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+  <cellXfs count="10">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="26" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="26" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -296,10 +261,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -326,116 +291,82 @@
         <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -447,363 +378,375 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28921E86-815C-4D28-B61B-DA9A063C903A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:AU18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="22" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="19.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="36" width="17.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="16.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="17.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="17.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="16.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="48" max="16384" width="9" style="1"/>
+    <col min="1" max="1" style="7" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="9" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="9" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="9" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="9" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="9" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="9" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="9" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="9" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="9" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="9" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="9" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="9" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="9" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="9" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="9" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="9" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="9" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="9" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="9" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="9" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="9" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="9" width="16.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="9" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="9" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="9" width="17.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="9" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="9" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="9" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="46" max="46" style="9" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="47" max="47" style="9" width="17.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="5" customFormat="1" ht="57" x14ac:dyDescent="0.4">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="AU1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI1" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AN1" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="AO1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AR1" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AS1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="AT1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="AU1" s="3" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2">
         <v>43830</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="3">
         <v>5</v>
       </c>
       <c r="C2" s="6">
@@ -942,11 +885,11 @@
         <v>-20765000</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="2">
         <v>43920</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="3">
         <v>7</v>
       </c>
       <c r="C3" s="6">
@@ -1037,13 +980,13 @@
         <v>0</v>
       </c>
       <c r="AF3" s="6">
-        <v>-5228672.1311475411</v>
+        <v>-5228672.131147541</v>
       </c>
       <c r="AG3" s="6">
-        <v>-6106918.0327868853</v>
+        <v>-6106918.032786885</v>
       </c>
       <c r="AH3" s="6">
-        <v>-3941196.7213114752</v>
+        <v>-3941196.721311475</v>
       </c>
       <c r="AI3" s="6">
         <v>-5685786.8852459015</v>
@@ -1052,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="AK3" s="6">
-        <v>-21117491.803278688</v>
+        <v>-21117491.80327869</v>
       </c>
       <c r="AL3" s="6">
         <v>-3085459.0163934426</v>
@@ -1073,7 +1016,7 @@
         <v>-20853885.245901637</v>
       </c>
       <c r="AR3" s="6">
-        <v>-98983.606557377061</v>
+        <v>-98983.60655737706</v>
       </c>
       <c r="AS3" s="6">
         <v>-20952868.852459017</v>
@@ -1085,11 +1028,11 @@
         <v>-20952868.852459017</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="2">
         <v>44012</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="3">
         <v>8</v>
       </c>
       <c r="C4" s="6">
@@ -1180,10 +1123,10 @@
         <v>0</v>
       </c>
       <c r="AF4" s="6">
-        <v>-6153448.0874316944</v>
+        <v>-6153448.087431694</v>
       </c>
       <c r="AG4" s="6">
-        <v>-5835945.3551912569</v>
+        <v>-5835945.355191257</v>
       </c>
       <c r="AH4" s="6">
         <v>-3637797.8142076503</v>
@@ -1195,7 +1138,7 @@
         <v>0</v>
       </c>
       <c r="AK4" s="6">
-        <v>-21547327.868852459</v>
+        <v>-21547327.86885246</v>
       </c>
       <c r="AL4" s="6">
         <v>-2045306.0109289617</v>
@@ -1228,11 +1171,11 @@
         <v>-21144912.56830601</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A5" s="7">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="2">
         <v>44104</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="3">
         <v>8</v>
       </c>
       <c r="C5" s="6">
@@ -1323,10 +1266,10 @@
         <v>0</v>
       </c>
       <c r="AF5" s="6">
-        <v>-7078224.0437158477</v>
+        <v>-7078224.043715848</v>
       </c>
       <c r="AG5" s="6">
-        <v>-5564972.6775956284</v>
+        <v>-5564972.677595628</v>
       </c>
       <c r="AH5" s="6">
         <v>-3334398.9071038254</v>
@@ -1338,7 +1281,7 @@
         <v>0</v>
       </c>
       <c r="AK5" s="6">
-        <v>-21977163.934426229</v>
+        <v>-21977163.93442623</v>
       </c>
       <c r="AL5" s="6">
         <v>-1005153.0054644808</v>
@@ -1371,11 +1314,11 @@
         <v>-21336956.284153007</v>
       </c>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A6" s="7">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+      <c r="A6" s="2">
         <v>44196</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="3">
         <v>18</v>
       </c>
       <c r="C6" s="6">
@@ -1514,11 +1457,11 @@
         <v>-21529000</v>
       </c>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A7" s="7">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="2">
         <v>44285</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="3">
         <v>18</v>
       </c>
       <c r="C7" s="6">
@@ -1543,13 +1486,13 @@
         <v>1734550.6849315069</v>
       </c>
       <c r="J7" s="6">
-        <v>27746687.671232879</v>
+        <v>27746687.67123288</v>
       </c>
       <c r="K7" s="6">
-        <v>53471972.602739729</v>
+        <v>53471972.60273973</v>
       </c>
       <c r="L7" s="6">
-        <v>3782624.6575342468</v>
+        <v>3782624.657534247</v>
       </c>
       <c r="M7" s="6">
         <v>121034402.73972602</v>
@@ -1564,10 +1507,10 @@
         <v>513909.58904109587</v>
       </c>
       <c r="Q7" s="6">
-        <v>572041.09589041094</v>
+        <v>572041.095890411</v>
       </c>
       <c r="R7" s="6">
-        <v>7666704.1095890412</v>
+        <v>7666704.109589041</v>
       </c>
       <c r="S7" s="6">
         <v>168495964.38356164</v>
@@ -1579,16 +1522,16 @@
         <v>1000000</v>
       </c>
       <c r="V7" s="6">
-        <v>649490.41095890407</v>
+        <v>649490.4109589041</v>
       </c>
       <c r="W7" s="6">
-        <v>200543030.13698629</v>
+        <v>200543030.1369863</v>
       </c>
       <c r="X7" s="6">
         <v>0</v>
       </c>
       <c r="Y7" s="6">
-        <v>69840402.739726022</v>
+        <v>69840402.73972602</v>
       </c>
       <c r="Z7" s="6">
         <v>0</v>
@@ -1600,7 +1543,7 @@
         <v>-152266219.1780822</v>
       </c>
       <c r="AC7" s="6">
-        <v>53471972.602739729</v>
+        <v>53471972.60273973</v>
       </c>
       <c r="AD7" s="6">
         <v>0</v>
@@ -1618,7 +1561,7 @@
         <v>-4907802.7397260275</v>
       </c>
       <c r="AI7" s="6">
-        <v>-7534526.0273972601</v>
+        <v>-7534526.02739726</v>
       </c>
       <c r="AJ7" s="6">
         <v>0</v>
@@ -1636,13 +1579,13 @@
         <v>0</v>
       </c>
       <c r="AO7" s="6">
-        <v>709821.91780821909</v>
+        <v>709821.9178082191</v>
       </c>
       <c r="AP7" s="6">
         <v>0</v>
       </c>
       <c r="AQ7" s="6">
-        <v>-39706709.589041099</v>
+        <v>-39706709.5890411</v>
       </c>
       <c r="AR7" s="6">
         <v>-55342.465753424665</v>
@@ -1657,11 +1600,11 @@
         <v>-39783021.91780822</v>
       </c>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A8" s="7">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25">
+      <c r="A8" s="2">
         <v>44377</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="3">
         <v>22</v>
       </c>
       <c r="C8" s="6">
@@ -1671,7 +1614,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="6">
-        <v>595101.36986301374</v>
+        <v>595101.3698630137</v>
       </c>
       <c r="F8" s="6">
         <v>1725597.2602739725</v>
@@ -1680,19 +1623,19 @@
         <v>15256591.780821918</v>
       </c>
       <c r="H8" s="6">
-        <v>33710624.657534249</v>
+        <v>33710624.65753425</v>
       </c>
       <c r="I8" s="6">
         <v>2141367.1232876712</v>
       </c>
       <c r="J8" s="6">
-        <v>18620791.780821919</v>
+        <v>18620791.78082192</v>
       </c>
       <c r="K8" s="6">
         <v>52287315.06849315</v>
       </c>
       <c r="L8" s="6">
-        <v>4738416.4383561648</v>
+        <v>4738416.438356165</v>
       </c>
       <c r="M8" s="6">
         <v>116847268.49315068</v>
@@ -1704,16 +1647,16 @@
         <v>0</v>
       </c>
       <c r="P8" s="6">
-        <v>670939.72602739721</v>
+        <v>670939.7260273972</v>
       </c>
       <c r="Q8" s="6">
-        <v>693027.39726027404</v>
+        <v>693027.397260274</v>
       </c>
       <c r="R8" s="6">
         <v>12922802.739726027</v>
       </c>
       <c r="S8" s="6">
-        <v>206902309.58904111</v>
+        <v>206902309.5890411</v>
       </c>
       <c r="T8" s="6">
         <v>1555197.2602739725</v>
@@ -1731,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="Y8" s="6">
-        <v>78717268.493150681</v>
+        <v>78717268.49315068</v>
       </c>
       <c r="Z8" s="6">
         <v>0</v>
@@ -1755,13 +1698,13 @@
         <v>-22203813.698630136</v>
       </c>
       <c r="AG8" s="6">
-        <v>-7447156.1643835623</v>
+        <v>-7447156.164383562</v>
       </c>
       <c r="AH8" s="6">
         <v>-6847868.493150685</v>
       </c>
       <c r="AI8" s="6">
-        <v>-9690350.6849315055</v>
+        <v>-9690350.684931505</v>
       </c>
       <c r="AJ8" s="6">
         <v>0</v>
@@ -1779,19 +1722,19 @@
         <v>0</v>
       </c>
       <c r="AO8" s="6">
-        <v>829547.94520547939</v>
+        <v>829547.9452054794</v>
       </c>
       <c r="AP8" s="6">
         <v>0</v>
       </c>
       <c r="AQ8" s="6">
-        <v>-58650139.726027399</v>
+        <v>-58650139.7260274</v>
       </c>
       <c r="AR8" s="6">
-        <v>40438.356164383556</v>
+        <v>40438.35616438356</v>
       </c>
       <c r="AS8" s="6">
-        <v>-58609701.369863011</v>
+        <v>-58609701.36986301</v>
       </c>
       <c r="AT8" s="6">
         <v>0</v>
@@ -1800,11 +1743,11 @@
         <v>-58652347.94520548</v>
       </c>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A9" s="7">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25">
+      <c r="A9" s="2">
         <v>44469</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="3">
         <v>22</v>
       </c>
       <c r="C9" s="6">
@@ -1814,7 +1757,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="6">
-        <v>895550.68493150687</v>
+        <v>895550.6849315069</v>
       </c>
       <c r="F9" s="6">
         <v>2210298.6301369863</v>
@@ -1829,13 +1772,13 @@
         <v>2548183.5616438356</v>
       </c>
       <c r="J9" s="6">
-        <v>9494895.8904109597</v>
+        <v>9494895.89041096</v>
       </c>
       <c r="K9" s="6">
-        <v>51102657.534246579</v>
+        <v>51102657.53424658</v>
       </c>
       <c r="L9" s="6">
-        <v>5694208.2191780824</v>
+        <v>5694208.219178082</v>
       </c>
       <c r="M9" s="6">
         <v>112660134.24657534</v>
@@ -1850,7 +1793,7 @@
         <v>827969.8630136986</v>
       </c>
       <c r="Q9" s="6">
-        <v>814013.69863013702</v>
+        <v>814013.698630137</v>
       </c>
       <c r="R9" s="6">
         <v>18178901.369863015</v>
@@ -1874,7 +1817,7 @@
         <v>0</v>
       </c>
       <c r="Y9" s="6">
-        <v>87594134.246575341</v>
+        <v>87594134.24657534</v>
       </c>
       <c r="Z9" s="6">
         <v>0</v>
@@ -1886,7 +1829,7 @@
         <v>-224580739.7260274</v>
       </c>
       <c r="AC9" s="6">
-        <v>51102657.534246579</v>
+        <v>51102657.53424658</v>
       </c>
       <c r="AD9" s="6">
         <v>0</v>
@@ -1898,10 +1841,10 @@
         <v>-29421906.84931507</v>
       </c>
       <c r="AG9" s="6">
-        <v>-8541578.0821917802</v>
+        <v>-8541578.08219178</v>
       </c>
       <c r="AH9" s="6">
-        <v>-8787934.2465753425</v>
+        <v>-8787934.246575342</v>
       </c>
       <c r="AI9" s="6">
         <v>-11846175.342465753</v>
@@ -1931,10 +1874,10 @@
         <v>-77593569.8630137</v>
       </c>
       <c r="AR9" s="6">
-        <v>136219.17808219179</v>
+        <v>136219.1780821918</v>
       </c>
       <c r="AS9" s="6">
-        <v>-77457350.684931502</v>
+        <v>-77457350.6849315</v>
       </c>
       <c r="AT9" s="6">
         <v>0</v>
@@ -1943,11 +1886,11 @@
         <v>-77521673.97260274</v>
       </c>
     </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25">
+      <c r="A10" s="2">
         <v>44561</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="3">
         <v>22</v>
       </c>
       <c r="C10" s="6">
@@ -2086,11 +2029,11 @@
         <v>-96391000</v>
       </c>
     </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A11" s="7">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="17.25">
+      <c r="A11" s="2">
         <v>44650</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="3">
         <v>22</v>
       </c>
       <c r="C11" s="6">
@@ -2103,25 +2046,25 @@
         <v>1242816.4383561644</v>
       </c>
       <c r="F11" s="6">
-        <v>2817649.3150684931</v>
+        <v>2817649.315068493</v>
       </c>
       <c r="G11" s="6">
-        <v>29203791.780821919</v>
+        <v>29203791.78082192</v>
       </c>
       <c r="H11" s="6">
         <v>36297504.10958904</v>
       </c>
       <c r="I11" s="6">
-        <v>4226846.5753424652</v>
+        <v>4226846.575342465</v>
       </c>
       <c r="J11" s="6">
         <v>1854934.2465753423</v>
       </c>
       <c r="K11" s="6">
-        <v>72823186.301369861</v>
+        <v>72823186.30136986</v>
       </c>
       <c r="L11" s="6">
-        <v>7430273.9726027399</v>
+        <v>7430273.97260274</v>
       </c>
       <c r="M11" s="6">
         <v>0</v>
@@ -2142,7 +2085,7 @@
         <v>19285405.479452055</v>
       </c>
       <c r="S11" s="6">
-        <v>221867802.73972601</v>
+        <v>221867802.739726</v>
       </c>
       <c r="T11" s="6">
         <v>3053465.7534246575</v>
@@ -2151,7 +2094,7 @@
         <v>1000000</v>
       </c>
       <c r="V11" s="6">
-        <v>2057013.6986301369</v>
+        <v>2057013.698630137</v>
       </c>
       <c r="W11" s="6">
         <v>227978282.19178084</v>
@@ -2163,7 +2106,7 @@
         <v>155346816.43835616</v>
       </c>
       <c r="Z11" s="6">
-        <v>-141106.84931506851</v>
+        <v>-141106.8493150685</v>
       </c>
       <c r="AA11" s="6">
         <v>-195108380.8219178</v>
@@ -2172,16 +2115,16 @@
         <v>-171265934.24657536</v>
       </c>
       <c r="AC11" s="6">
-        <v>72823186.301369861</v>
+        <v>72823186.30136986</v>
       </c>
       <c r="AD11" s="6">
-        <v>4677369.8630136987</v>
+        <v>4677369.863013699</v>
       </c>
       <c r="AE11" s="6">
         <v>-2219320.5479452056</v>
       </c>
       <c r="AF11" s="6">
-        <v>-36774353.424657539</v>
+        <v>-36774353.42465754</v>
       </c>
       <c r="AG11" s="6">
         <v>-10469673.97260274</v>
@@ -2190,16 +2133,16 @@
         <v>-11605320.547945205</v>
       </c>
       <c r="AI11" s="6">
-        <v>-17664654.794520549</v>
+        <v>-17664654.79452055</v>
       </c>
       <c r="AJ11" s="6">
-        <v>-78733323.287671238</v>
+        <v>-78733323.28767124</v>
       </c>
       <c r="AK11" s="6">
-        <v>-74055953.424657539</v>
+        <v>-74055953.42465754</v>
       </c>
       <c r="AL11" s="6">
-        <v>-7522509.5890410952</v>
+        <v>-7522509.589041095</v>
       </c>
       <c r="AM11" s="6">
         <v>27816402.739726026</v>
@@ -2211,33 +2154,33 @@
         <v>1086312.3287671234</v>
       </c>
       <c r="AP11" s="6">
-        <v>-6761208.2191780806</v>
+        <v>-6761208.219178081</v>
       </c>
       <c r="AQ11" s="6">
-        <v>-80817161.643835619</v>
+        <v>-80817161.64383562</v>
       </c>
       <c r="AR11" s="6">
-        <v>-939630.13698630151</v>
+        <v>-939630.1369863015</v>
       </c>
       <c r="AS11" s="6">
-        <v>-81756791.780821919</v>
+        <v>-81756791.78082192</v>
       </c>
       <c r="AT11" s="6">
         <v>-120136.98630136985</v>
       </c>
       <c r="AU11" s="6">
-        <v>-81876928.767123297</v>
+        <v>-81876928.7671233</v>
       </c>
     </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="17.25">
+      <c r="A12" s="2">
         <v>44742</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="3">
         <v>31</v>
       </c>
       <c r="C12" s="6">
-        <v>42251068.493150681</v>
+        <v>42251068.49315068</v>
       </c>
       <c r="D12" s="6">
         <v>0</v>
@@ -2249,34 +2192,34 @@
         <v>2944432.8767123288</v>
       </c>
       <c r="G12" s="6">
-        <v>46549194.520547949</v>
+        <v>46549194.52054795</v>
       </c>
       <c r="H12" s="6">
-        <v>40192002.739726029</v>
+        <v>40192002.73972603</v>
       </c>
       <c r="I12" s="6">
-        <v>5541564.3835616438</v>
+        <v>5541564.383561644</v>
       </c>
       <c r="J12" s="6">
         <v>3390956.1643835614</v>
       </c>
       <c r="K12" s="6">
-        <v>96500457.534246564</v>
+        <v>96500457.53424656</v>
       </c>
       <c r="L12" s="6">
-        <v>8236849.3150684927</v>
+        <v>8236849.315068493</v>
       </c>
       <c r="M12" s="6">
         <v>0</v>
       </c>
       <c r="N12" s="6">
-        <v>76340391.780821919</v>
+        <v>76340391.78082192</v>
       </c>
       <c r="O12" s="6">
         <v>0</v>
       </c>
       <c r="P12" s="6">
-        <v>1575605.4794520549</v>
+        <v>1575605.479452055</v>
       </c>
       <c r="Q12" s="6">
         <v>1433865.7534246575</v>
@@ -2300,10 +2243,10 @@
         <v>164537854.79452056</v>
       </c>
       <c r="X12" s="6">
-        <v>-90443175.342465758</v>
+        <v>-90443175.34246576</v>
       </c>
       <c r="Y12" s="6">
-        <v>216207210.95890409</v>
+        <v>216207210.9589041</v>
       </c>
       <c r="Z12" s="6">
         <v>-198071.23287671234</v>
@@ -2315,16 +2258,16 @@
         <v>-78777956.16438356</v>
       </c>
       <c r="AC12" s="6">
-        <v>96500457.534246564</v>
+        <v>96500457.53424656</v>
       </c>
       <c r="AD12" s="6">
-        <v>5122246.5753424661</v>
+        <v>5122246.575342466</v>
       </c>
       <c r="AE12" s="6">
-        <v>-2574213.6986301369</v>
+        <v>-2574213.698630137</v>
       </c>
       <c r="AF12" s="6">
-        <v>-36913235.616438359</v>
+        <v>-36913235.61643836</v>
       </c>
       <c r="AG12" s="6">
         <v>-11331449.315068493</v>
@@ -2339,13 +2282,13 @@
         <v>-84781882.19178082</v>
       </c>
       <c r="AK12" s="6">
-        <v>-79659635.616438359</v>
+        <v>-79659635.61643836</v>
       </c>
       <c r="AL12" s="6">
-        <v>-5232339.7260273974</v>
+        <v>-5232339.726027397</v>
       </c>
       <c r="AM12" s="6">
-        <v>37981268.493150681</v>
+        <v>37981268.49315068</v>
       </c>
       <c r="AN12" s="6">
         <v>0</v>
@@ -2357,57 +2300,57 @@
         <v>15092194.520547949</v>
       </c>
       <c r="AQ12" s="6">
-        <v>-64567441.095890418</v>
+        <v>-64567441.09589042</v>
       </c>
       <c r="AR12" s="6">
         <v>-2150753.4246575343</v>
       </c>
       <c r="AS12" s="6">
-        <v>-66718194.520547949</v>
+        <v>-66718194.52054795</v>
       </c>
       <c r="AT12" s="6">
         <v>-155424.65753424657</v>
       </c>
       <c r="AU12" s="6">
-        <v>-66873619.178082198</v>
+        <v>-66873619.1780822</v>
       </c>
     </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+      <c r="A13" s="2">
         <v>44834</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="3">
         <v>31</v>
       </c>
       <c r="C13" s="6">
-        <v>59389534.246575341</v>
+        <v>59389534.24657534</v>
       </c>
       <c r="D13" s="6">
         <v>0</v>
       </c>
       <c r="E13" s="6">
-        <v>1339605.4794520549</v>
+        <v>1339605.479452055</v>
       </c>
       <c r="F13" s="6">
         <v>3071216.4383561644</v>
       </c>
       <c r="G13" s="6">
-        <v>63894597.260273978</v>
+        <v>63894597.26027398</v>
       </c>
       <c r="H13" s="6">
-        <v>44086501.369863011</v>
+        <v>44086501.36986301</v>
       </c>
       <c r="I13" s="6">
-        <v>6856282.1917808224</v>
+        <v>6856282.191780822</v>
       </c>
       <c r="J13" s="6">
-        <v>4926978.0821917802</v>
+        <v>4926978.08219178</v>
       </c>
       <c r="K13" s="6">
         <v>120177728.76712328</v>
       </c>
       <c r="L13" s="6">
-        <v>9043424.6575342473</v>
+        <v>9043424.657534247</v>
       </c>
       <c r="M13" s="6">
         <v>0</v>
@@ -2428,10 +2371,10 @@
         <v>10706468.493150685</v>
       </c>
       <c r="S13" s="6">
-        <v>94003934.246575341</v>
+        <v>94003934.24657534</v>
       </c>
       <c r="T13" s="6">
-        <v>5059821.9178082198</v>
+        <v>5059821.91780822</v>
       </c>
       <c r="U13" s="6">
         <v>1000000</v>
@@ -2443,10 +2386,10 @@
         <v>101097427.39726028</v>
       </c>
       <c r="X13" s="6">
-        <v>-49523087.671232879</v>
+        <v>-49523087.67123288</v>
       </c>
       <c r="Y13" s="6">
-        <v>277067605.47945201</v>
+        <v>277067605.479452</v>
       </c>
       <c r="Z13" s="6">
         <v>-255035.61643835617</v>
@@ -2461,7 +2404,7 @@
         <v>120177728.76712328</v>
       </c>
       <c r="AD13" s="6">
-        <v>5567123.2876712326</v>
+        <v>5567123.287671233</v>
       </c>
       <c r="AE13" s="6">
         <v>-2929106.8493150687</v>
@@ -2479,7 +2422,7 @@
         <v>-25236884.93150685</v>
       </c>
       <c r="AJ13" s="6">
-        <v>-90830441.095890403</v>
+        <v>-90830441.0958904</v>
       </c>
       <c r="AK13" s="6">
         <v>-85263317.80821918</v>
@@ -2488,7 +2431,7 @@
         <v>-2942169.8630136987</v>
       </c>
       <c r="AM13" s="6">
-        <v>48146134.246575341</v>
+        <v>48146134.24657534</v>
       </c>
       <c r="AN13" s="6">
         <v>0</v>
@@ -2497,29 +2440,29 @@
         <v>1122104.1095890412</v>
       </c>
       <c r="AP13" s="6">
-        <v>36945597.260273978</v>
+        <v>36945597.26027398</v>
       </c>
       <c r="AQ13" s="6">
-        <v>-48317720.547945209</v>
+        <v>-48317720.54794521</v>
       </c>
       <c r="AR13" s="6">
         <v>-3361876.7123287674</v>
       </c>
       <c r="AS13" s="6">
-        <v>-51679597.260273978</v>
+        <v>-51679597.26027398</v>
       </c>
       <c r="AT13" s="6">
         <v>-190712.32876712328</v>
       </c>
       <c r="AU13" s="6">
-        <v>-51870309.589041099</v>
+        <v>-51870309.5890411</v>
       </c>
     </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A14" s="7">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="32.25">
+      <c r="A14" s="2">
         <v>44926</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="3">
         <v>31</v>
       </c>
       <c r="C14" s="6">
@@ -2658,11 +2601,11 @@
         <v>-36867000</v>
       </c>
     </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A15" s="7">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="32.25">
+      <c r="A15" s="2">
         <v>45015</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="3">
         <v>35</v>
       </c>
       <c r="C15" s="6">
@@ -2684,22 +2627,22 @@
         <v>46310482.19178082</v>
       </c>
       <c r="I15" s="6">
-        <v>6957673.9726027399</v>
+        <v>6957673.97260274</v>
       </c>
       <c r="J15" s="6">
-        <v>6229893.1506849313</v>
+        <v>6229893.150684931</v>
       </c>
       <c r="K15" s="6">
         <v>127402679.4520548</v>
       </c>
       <c r="L15" s="6">
-        <v>9383054.7945205476</v>
+        <v>9383054.794520548</v>
       </c>
       <c r="M15" s="6">
         <v>0</v>
       </c>
       <c r="N15" s="6">
-        <v>6984150.6849315073</v>
+        <v>6984150.684931507</v>
       </c>
       <c r="O15" s="6">
         <v>1125257.5342465753</v>
@@ -2711,13 +2654,13 @@
         <v>2376734.2465753425</v>
       </c>
       <c r="R15" s="6">
-        <v>5918356.1643835614</v>
+        <v>5918356.164383561</v>
       </c>
       <c r="S15" s="6">
         <v>27955506.84931507</v>
       </c>
       <c r="T15" s="6">
-        <v>5020846.5753424652</v>
+        <v>5020846.575342465</v>
       </c>
       <c r="U15" s="6">
         <v>1000000</v>
@@ -2726,13 +2669,13 @@
         <v>522975.34246575343</v>
       </c>
       <c r="W15" s="6">
-        <v>34499328.767123289</v>
+        <v>34499328.76712329</v>
       </c>
       <c r="X15" s="6">
         <v>-8603000</v>
       </c>
       <c r="Y15" s="6">
-        <v>339443682.19178081</v>
+        <v>339443682.1917808</v>
       </c>
       <c r="Z15" s="6">
         <v>-243969.86301369863</v>
@@ -2741,19 +2684,19 @@
         <v>-237693361.6438356</v>
       </c>
       <c r="AB15" s="6">
-        <v>92903350.684931517</v>
+        <v>92903350.68493152</v>
       </c>
       <c r="AC15" s="6">
         <v>127402679.4520548</v>
       </c>
       <c r="AD15" s="6">
-        <v>7002460.2739726026</v>
+        <v>7002460.273972603</v>
       </c>
       <c r="AE15" s="6">
-        <v>-3716076.7123287669</v>
+        <v>-3716076.712328767</v>
       </c>
       <c r="AF15" s="6">
-        <v>-33852646.575342469</v>
+        <v>-33852646.57534247</v>
       </c>
       <c r="AG15" s="6">
         <v>-12470038.356164385</v>
@@ -2765,13 +2708,13 @@
         <v>-27556572.602739725</v>
       </c>
       <c r="AJ15" s="6">
-        <v>-92635772.602739722</v>
+        <v>-92635772.60273972</v>
       </c>
       <c r="AK15" s="6">
-        <v>-85633312.328767121</v>
+        <v>-85633312.32876712</v>
       </c>
       <c r="AL15" s="6">
-        <v>-73134.246575342375</v>
+        <v>-73134.24657534237</v>
       </c>
       <c r="AM15" s="6">
         <v>45671293.15068493</v>
@@ -2780,16 +2723,16 @@
         <v>0</v>
       </c>
       <c r="AO15" s="6">
-        <v>3122627.3972602738</v>
+        <v>3122627.397260274</v>
       </c>
       <c r="AP15" s="6">
-        <v>48720786.301369861</v>
+        <v>48720786.30136986</v>
       </c>
       <c r="AQ15" s="6">
         <v>-36912526.02739726</v>
       </c>
       <c r="AR15" s="6">
-        <v>-5672454.7945205476</v>
+        <v>-5672454.794520548</v>
       </c>
       <c r="AS15" s="6">
         <v>-42584980.82191781</v>
@@ -2801,11 +2744,11 @@
         <v>-42687843.83561644</v>
       </c>
     </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A16" s="7">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="32.25">
+      <c r="A16" s="2">
         <v>45107</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="3">
         <v>43</v>
       </c>
       <c r="C16" s="6">
@@ -2818,55 +2761,55 @@
         <v>1146501.3698630137</v>
       </c>
       <c r="F16" s="6">
-        <v>2689712.3287671232</v>
+        <v>2689712.328767123</v>
       </c>
       <c r="G16" s="6">
-        <v>54119753.424657539</v>
+        <v>54119753.42465754</v>
       </c>
       <c r="H16" s="6">
-        <v>44583654.794520549</v>
+        <v>44583654.79452055</v>
       </c>
       <c r="I16" s="6">
-        <v>5703449.3150684927</v>
+        <v>5703449.315068493</v>
       </c>
       <c r="J16" s="6">
-        <v>5988928.7671232875</v>
+        <v>5988928.767123288</v>
       </c>
       <c r="K16" s="6">
         <v>110395786.30136986</v>
       </c>
       <c r="L16" s="6">
-        <v>8900369.8630136978</v>
+        <v>8900369.863013698</v>
       </c>
       <c r="M16" s="6">
         <v>0</v>
       </c>
       <c r="N16" s="6">
-        <v>5587767.1232876712</v>
+        <v>5587767.123287671</v>
       </c>
       <c r="O16" s="6">
-        <v>889838.35616438359</v>
+        <v>889838.3561643836</v>
       </c>
       <c r="P16" s="6">
-        <v>2159635.6164383562</v>
+        <v>2159635.616438356</v>
       </c>
       <c r="Q16" s="6">
-        <v>2827156.1643835618</v>
+        <v>2827156.164383562</v>
       </c>
       <c r="R16" s="6">
-        <v>5402904.1095890412</v>
+        <v>5402904.109589041</v>
       </c>
       <c r="S16" s="6">
-        <v>25767671.232876711</v>
+        <v>25767671.23287671</v>
       </c>
       <c r="T16" s="6">
-        <v>3943564.3835616438</v>
+        <v>3943564.383561644</v>
       </c>
       <c r="U16" s="6">
         <v>1000000</v>
       </c>
       <c r="V16" s="6">
-        <v>523983.56164383562</v>
+        <v>523983.5616438356</v>
       </c>
       <c r="W16" s="6">
         <v>31235219.17808219</v>
@@ -2884,16 +2827,16 @@
         <v>-253073241.0958904</v>
       </c>
       <c r="AB16" s="6">
-        <v>79160567.123287678</v>
+        <v>79160567.12328768</v>
       </c>
       <c r="AC16" s="6">
         <v>110395786.30136986</v>
       </c>
       <c r="AD16" s="6">
-        <v>8026306.8493150687</v>
+        <v>8026306.849315069</v>
       </c>
       <c r="AE16" s="6">
-        <v>-4162717.8082191781</v>
+        <v>-4162717.808219178</v>
       </c>
       <c r="AF16" s="6">
         <v>-30401764.383561645</v>
@@ -2908,34 +2851,34 @@
         <v>-26040715.06849315</v>
       </c>
       <c r="AJ16" s="6">
-        <v>-88249515.068493158</v>
+        <v>-88249515.06849316</v>
       </c>
       <c r="AK16" s="6">
-        <v>-80223208.219178081</v>
+        <v>-80223208.21917808</v>
       </c>
       <c r="AL16" s="6">
-        <v>525243.83561643842</v>
+        <v>525243.8356164384</v>
       </c>
       <c r="AM16" s="6">
-        <v>32605528.767123289</v>
+        <v>32605528.76712329</v>
       </c>
       <c r="AN16" s="6">
         <v>0</v>
       </c>
       <c r="AO16" s="6">
-        <v>5172084.9315068498</v>
+        <v>5172084.93150685</v>
       </c>
       <c r="AP16" s="6">
-        <v>38302857.534246579</v>
+        <v>38302857.53424658</v>
       </c>
       <c r="AQ16" s="6">
-        <v>-41920350.684931509</v>
+        <v>-41920350.68493151</v>
       </c>
       <c r="AR16" s="6">
-        <v>-6808969.8630136987</v>
+        <v>-6808969.863013699</v>
       </c>
       <c r="AS16" s="6">
-        <v>-48729320.547945209</v>
+        <v>-48729320.54794521</v>
       </c>
       <c r="AT16" s="6">
         <v>24424.657534246566</v>
@@ -2944,11 +2887,11 @@
         <v>-48704895.89041096</v>
       </c>
     </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A17" s="7">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="32.25">
+      <c r="A17" s="2">
         <v>45199</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="3">
         <v>43</v>
       </c>
       <c r="C17" s="6">
@@ -2961,25 +2904,25 @@
         <v>1023750.6849315069</v>
       </c>
       <c r="F17" s="6">
-        <v>2431356.1643835618</v>
+        <v>2431356.164383562</v>
       </c>
       <c r="G17" s="6">
-        <v>40334876.712328769</v>
+        <v>40334876.71232877</v>
       </c>
       <c r="H17" s="6">
-        <v>42856827.397260278</v>
+        <v>42856827.39726028</v>
       </c>
       <c r="I17" s="6">
-        <v>4449224.6575342463</v>
+        <v>4449224.657534246</v>
       </c>
       <c r="J17" s="6">
-        <v>5747964.3835616438</v>
+        <v>5747964.383561644</v>
       </c>
       <c r="K17" s="6">
-        <v>93388893.150684923</v>
+        <v>93388893.15068492</v>
       </c>
       <c r="L17" s="6">
-        <v>8417684.9315068498</v>
+        <v>8417684.93150685</v>
       </c>
       <c r="M17" s="6">
         <v>0</v>
@@ -2988,28 +2931,28 @@
         <v>4191383.5616438356</v>
       </c>
       <c r="O17" s="6">
-        <v>654419.17808219185</v>
+        <v>654419.1780821919</v>
       </c>
       <c r="P17" s="6">
-        <v>2151317.8082191781</v>
+        <v>2151317.808219178</v>
       </c>
       <c r="Q17" s="6">
-        <v>3277578.0821917811</v>
+        <v>3277578.082191781</v>
       </c>
       <c r="R17" s="6">
-        <v>4887452.0547945211</v>
+        <v>4887452.054794521</v>
       </c>
       <c r="S17" s="6">
         <v>23579835.616438355</v>
       </c>
       <c r="T17" s="6">
-        <v>2866282.1917808219</v>
+        <v>2866282.191780822</v>
       </c>
       <c r="U17" s="6">
         <v>1000000</v>
       </c>
       <c r="V17" s="6">
-        <v>524991.78082191781</v>
+        <v>524991.7808219178</v>
       </c>
       <c r="W17" s="6">
         <v>27971109.589041095</v>
@@ -3018,7 +2961,7 @@
         <v>-8603000</v>
       </c>
       <c r="Y17" s="6">
-        <v>342577227.39726031</v>
+        <v>342577227.3972603</v>
       </c>
       <c r="Z17" s="6">
         <v>-103323.28767123287</v>
@@ -3027,16 +2970,16 @@
         <v>-268453120.5479452</v>
       </c>
       <c r="AB17" s="6">
-        <v>65417783.561643839</v>
+        <v>65417783.56164384</v>
       </c>
       <c r="AC17" s="6">
-        <v>93388893.150684923</v>
+        <v>93388893.15068492</v>
       </c>
       <c r="AD17" s="6">
-        <v>9050153.4246575348</v>
+        <v>9050153.424657535</v>
       </c>
       <c r="AE17" s="6">
-        <v>-4609358.9041095888</v>
+        <v>-4609358.904109589</v>
       </c>
       <c r="AF17" s="6">
         <v>-26950882.19178082</v>
@@ -3051,7 +2994,7 @@
         <v>-24524857.534246575</v>
       </c>
       <c r="AJ17" s="6">
-        <v>-83863257.534246579</v>
+        <v>-83863257.53424658</v>
       </c>
       <c r="AK17" s="6">
         <v>-74813104.10958904</v>
@@ -3066,19 +3009,19 @@
         <v>0</v>
       </c>
       <c r="AO17" s="6">
-        <v>7221542.4657534249</v>
+        <v>7221542.465753425</v>
       </c>
       <c r="AP17" s="6">
-        <v>27884928.767123289</v>
+        <v>27884928.76712329</v>
       </c>
       <c r="AQ17" s="6">
-        <v>-46928175.342465758</v>
+        <v>-46928175.34246576</v>
       </c>
       <c r="AR17" s="6">
-        <v>-7945484.9315068498</v>
+        <v>-7945484.93150685</v>
       </c>
       <c r="AS17" s="6">
-        <v>-54873660.273972601</v>
+        <v>-54873660.2739726</v>
       </c>
       <c r="AT17" s="6">
         <v>151712.32876712328</v>
@@ -3087,11 +3030,11 @@
         <v>-54721947.94520548</v>
       </c>
     </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A18" s="7">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="32.25">
+      <c r="A18" s="2">
         <v>45291</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="3">
         <v>43</v>
       </c>
       <c r="C18" s="6">
@@ -3231,8 +3174,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>